<commit_message>
RQ2 first 150 commit manual analysis
</commit_message>
<xml_diff>
--- a/RQ2_Commit_Manual_Analysis_Tejas.xlsx
+++ b/RQ2_Commit_Manual_Analysis_Tejas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Thesis\CPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB10F807-A37C-4CCF-BD25-75ECEA5A28AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69517D9-6A98-4C00-BE26-E19619C207CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="458">
   <si>
     <t>Table 1</t>
   </si>
@@ -1290,18 +1290,6 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>https://github.com/OpenDroneMap/WebODM/commit/a5aa6069a1168a074c52c0cf29fdc2c9c1cab491</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
       <t>https://github.com/OpenDroneMap/WebODM/commit/b185c775841e126749545b7f85d24fbea1b6e4ac</t>
     </r>
   </si>
@@ -1398,18 +1386,6 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>https://github.com/alexa/alexa-auto-sdk/commit/1cf7062511253b674099665a0c6fc5b1d3f5918c</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
       <t>https://github.com/apache/nuttx/commit/155c9a20705f383144dd49d75decc5def193556a</t>
     </r>
   </si>
@@ -1422,18 +1398,6 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>https://github.com/apache/nuttx/commit/1bd0e0ec9194966c41b3eab666e5070c61a28419</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
       <t>https://github.com/apache/nuttx/commit/25bd3be1678feea1c846267adbe64656d22eb91d</t>
     </r>
   </si>
@@ -4061,6 +4025,66 @@
   </si>
   <si>
     <t>install dependancy and deletes the header files</t>
+  </si>
+  <si>
+    <t>removed "/" from file and added run command in script.</t>
+  </si>
+  <si>
+    <t>removed the location of build content and added new service in docker-compose.yml file.</t>
+  </si>
+  <si>
+    <t>add extxra command for changing the permission of script. Add two new environment in docker-compose.yml file.</t>
+  </si>
+  <si>
+    <t>added a submodule in docker.yml</t>
+  </si>
+  <si>
+    <t>Install postgresql client .Added a extra command for "--quiet" to suppresses most output and only shows errors.</t>
+  </si>
+  <si>
+    <t>Added a new envrionment variable</t>
+  </si>
+  <si>
+    <t>Added a new port to host application</t>
+  </si>
+  <si>
+    <t>https://github.com/OpenDroneMap/WebODM/commit/a5aa6069a1168a074c52c0cf29fdc2c9c1cab491</t>
+  </si>
+  <si>
+    <t>Adds a check for linux sysemd service to start webodm-gunicorn.service in short acts a hard dependency</t>
+  </si>
+  <si>
+    <t>same command but used step by step</t>
+  </si>
+  <si>
+    <t>replaced building packages with just read command</t>
+  </si>
+  <si>
+    <t>add command for installing webpack-cli</t>
+  </si>
+  <si>
+    <t>added a new installation package of libgdal-dev and install numpy library</t>
+  </si>
+  <si>
+    <t>changed the link to install different version of android-ndk</t>
+  </si>
+  <si>
+    <t>upgraded the pip version before installing whell and pre-commit</t>
+  </si>
+  <si>
+    <t>https://github.com/alexa/alexa-auto-sdk/commit/1cf7062511253b674099665a0c6fc5b1d3f5918c</t>
+  </si>
+  <si>
+    <t>743 files changed but no change in docker files, just changes for building application.</t>
+  </si>
+  <si>
+    <t>changes in github actions</t>
+  </si>
+  <si>
+    <t>https://github.com/apache/nuttx/commit/1bd0e0ec9194966c41b3eab666e5070c61a28419</t>
+  </si>
+  <si>
+    <t>added environment variables, install linux-x86_64</t>
   </si>
 </sst>
 </file>
@@ -5468,8 +5492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H335"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B126" workbookViewId="0">
-      <selection activeCell="B134" sqref="B134"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B140" workbookViewId="0">
+      <selection activeCell="B151" sqref="B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
@@ -5517,7 +5541,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -5533,7 +5557,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -5549,7 +5573,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -5565,7 +5589,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -5581,7 +5605,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -5597,7 +5621,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
@@ -5613,7 +5637,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -5629,7 +5653,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -5645,7 +5669,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
@@ -5661,7 +5685,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
@@ -5674,10 +5698,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
@@ -5693,7 +5717,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
@@ -5709,7 +5733,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
@@ -5725,7 +5749,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
@@ -5741,7 +5765,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
@@ -5757,7 +5781,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
@@ -5773,7 +5797,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
@@ -5789,7 +5813,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
@@ -5805,7 +5829,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
@@ -5821,7 +5845,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
@@ -5837,7 +5861,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
@@ -5853,7 +5877,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
@@ -5869,7 +5893,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
@@ -5882,10 +5906,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
@@ -5901,7 +5925,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
@@ -5917,7 +5941,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
@@ -5933,7 +5957,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
@@ -5949,7 +5973,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
@@ -5962,10 +5986,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
@@ -5981,7 +6005,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
@@ -5997,7 +6021,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
@@ -6010,10 +6034,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
@@ -6043,7 +6067,7 @@
         <v>33</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
@@ -6059,7 +6083,7 @@
         <v>34</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
@@ -6075,7 +6099,7 @@
         <v>35</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
@@ -6091,7 +6115,7 @@
         <v>36</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
@@ -6104,10 +6128,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
@@ -6123,7 +6147,7 @@
         <v>37</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
@@ -6139,7 +6163,7 @@
         <v>38</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
@@ -6155,7 +6179,7 @@
         <v>39</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
@@ -6171,7 +6195,7 @@
         <v>40</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
@@ -6187,7 +6211,7 @@
         <v>41</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
@@ -6203,7 +6227,7 @@
         <v>42</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
@@ -6216,10 +6240,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
@@ -6235,7 +6259,7 @@
         <v>43</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -6251,7 +6275,7 @@
         <v>44</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
@@ -6267,7 +6291,7 @@
         <v>45</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
@@ -6283,7 +6307,7 @@
         <v>46</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
@@ -6299,7 +6323,7 @@
         <v>47</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
@@ -6312,10 +6336,10 @@
         <v>51</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
@@ -6331,7 +6355,7 @@
         <v>48</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D54" s="11"/>
       <c r="E54" s="11"/>
@@ -6347,7 +6371,7 @@
         <v>49</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D55" s="11"/>
       <c r="E55" s="11"/>
@@ -6363,7 +6387,7 @@
         <v>50</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D56" s="11"/>
       <c r="E56" s="11"/>
@@ -6379,7 +6403,7 @@
         <v>51</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
@@ -6395,7 +6419,7 @@
         <v>52</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
@@ -6411,7 +6435,7 @@
         <v>53</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D59" s="11"/>
       <c r="E59" s="11"/>
@@ -6427,7 +6451,7 @@
         <v>54</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
@@ -6443,7 +6467,7 @@
         <v>55</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
@@ -6456,10 +6480,10 @@
         <v>60</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
@@ -6475,7 +6499,7 @@
         <v>56</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
@@ -6488,10 +6512,10 @@
         <v>62</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
@@ -6504,10 +6528,10 @@
         <v>63</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
@@ -6523,7 +6547,7 @@
         <v>57</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D66" s="11"/>
       <c r="E66" s="11"/>
@@ -6539,7 +6563,7 @@
         <v>58</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D67" s="11"/>
       <c r="E67" s="11"/>
@@ -6555,7 +6579,7 @@
         <v>59</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
@@ -6571,7 +6595,7 @@
         <v>60</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
@@ -6587,7 +6611,7 @@
         <v>61</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
@@ -6600,10 +6624,10 @@
         <v>69</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D71" s="11"/>
       <c r="E71" s="11"/>
@@ -6619,7 +6643,7 @@
         <v>62</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
@@ -6635,7 +6659,7 @@
         <v>63</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
@@ -6648,10 +6672,10 @@
         <v>72</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D74" s="11"/>
       <c r="E74" s="11"/>
@@ -6664,10 +6688,10 @@
         <v>73</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D75" s="11"/>
       <c r="E75" s="11"/>
@@ -6683,7 +6707,7 @@
         <v>64</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
@@ -6699,7 +6723,7 @@
         <v>65</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
@@ -6715,7 +6739,7 @@
         <v>66</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
@@ -6728,10 +6752,10 @@
         <v>77</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
@@ -6744,10 +6768,10 @@
         <v>78</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
@@ -6760,10 +6784,10 @@
         <v>79</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
@@ -6779,7 +6803,7 @@
         <v>67</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D82" s="11"/>
       <c r="E82" s="11"/>
@@ -6795,7 +6819,7 @@
         <v>68</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D83" s="11"/>
       <c r="E83" s="11"/>
@@ -6811,7 +6835,7 @@
         <v>69</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D84" s="11"/>
       <c r="E84" s="11"/>
@@ -6827,7 +6851,7 @@
         <v>70</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D85" s="11"/>
       <c r="E85" s="11"/>
@@ -6843,7 +6867,7 @@
         <v>71</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
@@ -6859,7 +6883,7 @@
         <v>72</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
@@ -6875,7 +6899,7 @@
         <v>73</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
@@ -6888,10 +6912,10 @@
         <v>87</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
@@ -6904,10 +6928,10 @@
         <v>88</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
@@ -6920,10 +6944,10 @@
         <v>89</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
@@ -6939,7 +6963,7 @@
         <v>74</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
@@ -6952,10 +6976,10 @@
         <v>91</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
@@ -6968,10 +6992,10 @@
         <v>92</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
@@ -6987,7 +7011,7 @@
         <v>75</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
@@ -7003,7 +7027,7 @@
         <v>76</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
@@ -7016,10 +7040,10 @@
         <v>95</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
@@ -7035,7 +7059,7 @@
         <v>77</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
@@ -7048,10 +7072,10 @@
         <v>97</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
@@ -7064,10 +7088,10 @@
         <v>98</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
@@ -7083,7 +7107,7 @@
         <v>78</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D101" s="11"/>
       <c r="E101" s="11"/>
@@ -7099,7 +7123,7 @@
         <v>79</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
@@ -7115,7 +7139,7 @@
         <v>80</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
@@ -7128,10 +7152,10 @@
         <v>102</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D104" s="11"/>
       <c r="E104" s="11"/>
@@ -7147,7 +7171,7 @@
         <v>81</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
@@ -7163,7 +7187,7 @@
         <v>82</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
@@ -7176,10 +7200,10 @@
         <v>105</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
@@ -7195,7 +7219,7 @@
         <v>83</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
@@ -7211,7 +7235,7 @@
         <v>84</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D109" s="11"/>
       <c r="E109" s="11"/>
@@ -7224,10 +7248,10 @@
         <v>108</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D110" s="11"/>
       <c r="E110" s="11"/>
@@ -7243,7 +7267,7 @@
         <v>85</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D111" s="11"/>
       <c r="E111" s="11"/>
@@ -7259,7 +7283,7 @@
         <v>86</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D112" s="11"/>
       <c r="E112" s="11"/>
@@ -7275,7 +7299,7 @@
         <v>87</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D113" s="11"/>
       <c r="E113" s="11"/>
@@ -7291,7 +7315,7 @@
         <v>88</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D114" s="11"/>
       <c r="E114" s="11"/>
@@ -7304,10 +7328,10 @@
         <v>113</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D115" s="11"/>
       <c r="E115" s="11"/>
@@ -7323,7 +7347,7 @@
         <v>89</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D116" s="11"/>
       <c r="E116" s="11"/>
@@ -7339,7 +7363,7 @@
         <v>90</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D117" s="11"/>
       <c r="E117" s="11"/>
@@ -7355,7 +7379,7 @@
         <v>91</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D118" s="11"/>
       <c r="E118" s="11"/>
@@ -7371,7 +7395,7 @@
         <v>92</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D119" s="11"/>
       <c r="E119" s="11"/>
@@ -7387,7 +7411,7 @@
         <v>93</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D120" s="11"/>
       <c r="E120" s="11"/>
@@ -7403,7 +7427,7 @@
         <v>94</v>
       </c>
       <c r="C121" s="12" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D121" s="11"/>
       <c r="E121" s="11"/>
@@ -7416,10 +7440,10 @@
         <v>120</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C122" s="12" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D122" s="11"/>
       <c r="E122" s="11"/>
@@ -7435,7 +7459,7 @@
         <v>95</v>
       </c>
       <c r="C123" s="12" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D123" s="11"/>
       <c r="E123" s="11"/>
@@ -7451,7 +7475,7 @@
         <v>96</v>
       </c>
       <c r="C124" s="12" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D124" s="11"/>
       <c r="E124" s="11"/>
@@ -7467,7 +7491,7 @@
         <v>97</v>
       </c>
       <c r="C125" s="12" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D125" s="11"/>
       <c r="E125" s="11"/>
@@ -7480,10 +7504,10 @@
         <v>124</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C126" s="12" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D126" s="11"/>
       <c r="E126" s="11"/>
@@ -7499,7 +7523,7 @@
         <v>98</v>
       </c>
       <c r="C127" s="12" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D127" s="11"/>
       <c r="E127" s="11"/>
@@ -7515,7 +7539,7 @@
         <v>99</v>
       </c>
       <c r="C128" s="12" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D128" s="11"/>
       <c r="E128" s="11"/>
@@ -7528,9 +7552,11 @@
         <v>127</v>
       </c>
       <c r="B129" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="C129" s="12" t="s">
         <v>438</v>
       </c>
-      <c r="C129" s="12"/>
       <c r="D129" s="11"/>
       <c r="E129" s="11"/>
       <c r="F129" s="11"/>
@@ -7544,7 +7570,9 @@
       <c r="B130" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C130" s="12"/>
+      <c r="C130" s="12" t="s">
+        <v>439</v>
+      </c>
       <c r="D130" s="11"/>
       <c r="E130" s="11"/>
       <c r="F130" s="11"/>
@@ -7558,7 +7586,9 @@
       <c r="B131" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C131" s="12"/>
+      <c r="C131" s="12" t="s">
+        <v>362</v>
+      </c>
       <c r="D131" s="11"/>
       <c r="E131" s="11"/>
       <c r="F131" s="11"/>
@@ -7572,7 +7602,9 @@
       <c r="B132" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C132" s="12"/>
+      <c r="C132" s="12" t="s">
+        <v>440</v>
+      </c>
       <c r="D132" s="11"/>
       <c r="E132" s="11"/>
       <c r="F132" s="11"/>
@@ -7586,7 +7618,9 @@
       <c r="B133" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C133" s="12"/>
+      <c r="C133" s="12" t="s">
+        <v>441</v>
+      </c>
       <c r="D133" s="11"/>
       <c r="E133" s="11"/>
       <c r="F133" s="11"/>
@@ -7600,7 +7634,9 @@
       <c r="B134" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C134" s="12"/>
+      <c r="C134" s="12" t="s">
+        <v>442</v>
+      </c>
       <c r="D134" s="11"/>
       <c r="E134" s="11"/>
       <c r="F134" s="11"/>
@@ -7614,7 +7650,9 @@
       <c r="B135" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C135" s="12"/>
+      <c r="C135" s="12" t="s">
+        <v>318</v>
+      </c>
       <c r="D135" s="11"/>
       <c r="E135" s="11"/>
       <c r="F135" s="11"/>
@@ -7628,7 +7666,9 @@
       <c r="B136" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C136" s="12"/>
+      <c r="C136" s="12" t="s">
+        <v>443</v>
+      </c>
       <c r="D136" s="11"/>
       <c r="E136" s="11"/>
       <c r="F136" s="11"/>
@@ -7642,7 +7682,9 @@
       <c r="B137" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C137" s="12"/>
+      <c r="C137" s="12" t="s">
+        <v>444</v>
+      </c>
       <c r="D137" s="11"/>
       <c r="E137" s="11"/>
       <c r="F137" s="11"/>
@@ -7653,10 +7695,12 @@
       <c r="A138" s="8">
         <v>136</v>
       </c>
-      <c r="B138" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C138" s="10"/>
+      <c r="B138" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="C138" s="10" t="s">
+        <v>446</v>
+      </c>
       <c r="D138" s="11"/>
       <c r="E138" s="11"/>
       <c r="F138" s="11"/>
@@ -7668,9 +7712,11 @@
         <v>137</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="C139" s="12"/>
+        <v>108</v>
+      </c>
+      <c r="C139" s="12" t="s">
+        <v>447</v>
+      </c>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
       <c r="F139" s="11"/>
@@ -7682,9 +7728,11 @@
         <v>138</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C140" s="12"/>
+        <v>109</v>
+      </c>
+      <c r="C140" s="12" t="s">
+        <v>448</v>
+      </c>
       <c r="D140" s="11"/>
       <c r="E140" s="11"/>
       <c r="F140" s="11"/>
@@ -7696,9 +7744,11 @@
         <v>139</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C141" s="12"/>
+        <v>110</v>
+      </c>
+      <c r="C141" s="12" t="s">
+        <v>449</v>
+      </c>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
       <c r="F141" s="11"/>
@@ -7710,9 +7760,11 @@
         <v>140</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C142" s="12"/>
+        <v>111</v>
+      </c>
+      <c r="C142" s="12" t="s">
+        <v>450</v>
+      </c>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
       <c r="F142" s="11"/>
@@ -7724,9 +7776,11 @@
         <v>141</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="C143" s="12"/>
+        <v>112</v>
+      </c>
+      <c r="C143" s="12" t="s">
+        <v>451</v>
+      </c>
       <c r="D143" s="11"/>
       <c r="E143" s="11"/>
       <c r="F143" s="11"/>
@@ -7738,9 +7792,11 @@
         <v>142</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C144" s="12"/>
+        <v>113</v>
+      </c>
+      <c r="C144" s="12" t="s">
+        <v>452</v>
+      </c>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
       <c r="F144" s="11"/>
@@ -7752,9 +7808,11 @@
         <v>143</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C145" s="12"/>
+        <v>114</v>
+      </c>
+      <c r="C145" s="12" t="s">
+        <v>404</v>
+      </c>
       <c r="D145" s="11"/>
       <c r="E145" s="11"/>
       <c r="F145" s="11"/>
@@ -7766,9 +7824,11 @@
         <v>144</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C146" s="12"/>
+        <v>115</v>
+      </c>
+      <c r="C146" s="12" t="s">
+        <v>404</v>
+      </c>
       <c r="D146" s="11"/>
       <c r="E146" s="11"/>
       <c r="F146" s="11"/>
@@ -7779,10 +7839,12 @@
       <c r="A147" s="8">
         <v>145</v>
       </c>
-      <c r="B147" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C147" s="12"/>
+      <c r="B147" s="13" t="s">
+        <v>453</v>
+      </c>
+      <c r="C147" s="12" t="s">
+        <v>454</v>
+      </c>
       <c r="D147" s="11"/>
       <c r="E147" s="11"/>
       <c r="F147" s="11"/>
@@ -7794,9 +7856,11 @@
         <v>146</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C148" s="12"/>
+        <v>116</v>
+      </c>
+      <c r="C148" s="12" t="s">
+        <v>455</v>
+      </c>
       <c r="D148" s="11"/>
       <c r="E148" s="11"/>
       <c r="F148" s="11"/>
@@ -7807,10 +7871,12 @@
       <c r="A149" s="8">
         <v>147</v>
       </c>
-      <c r="B149" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C149" s="12"/>
+      <c r="B149" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="C149" s="12" t="s">
+        <v>318</v>
+      </c>
       <c r="D149" s="11"/>
       <c r="E149" s="11"/>
       <c r="F149" s="11"/>
@@ -7822,9 +7888,11 @@
         <v>148</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C150" s="12"/>
+        <v>117</v>
+      </c>
+      <c r="C150" s="12" t="s">
+        <v>457</v>
+      </c>
       <c r="D150" s="11"/>
       <c r="E150" s="11"/>
       <c r="F150" s="11"/>
@@ -7836,7 +7904,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C151" s="12"/>
       <c r="D151" s="11"/>
@@ -7850,7 +7918,7 @@
         <v>150</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C152" s="12"/>
       <c r="D152" s="11"/>
@@ -7864,7 +7932,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C153" s="12"/>
       <c r="D153" s="11"/>
@@ -7878,7 +7946,7 @@
         <v>152</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C154" s="12"/>
       <c r="D154" s="11"/>
@@ -7892,7 +7960,7 @@
         <v>153</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C155" s="12"/>
       <c r="D155" s="11"/>
@@ -7906,7 +7974,7 @@
         <v>154</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C156" s="12"/>
       <c r="D156" s="11"/>
@@ -7920,7 +7988,7 @@
         <v>155</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C157" s="12"/>
       <c r="D157" s="11"/>
@@ -7934,7 +8002,7 @@
         <v>156</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C158" s="12"/>
       <c r="D158" s="11"/>
@@ -7948,7 +8016,7 @@
         <v>157</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C159" s="12"/>
       <c r="D159" s="11"/>
@@ -7962,7 +8030,7 @@
         <v>158</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C160" s="12"/>
       <c r="D160" s="11"/>
@@ -7976,7 +8044,7 @@
         <v>159</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C161" s="12"/>
       <c r="D161" s="11"/>
@@ -7990,7 +8058,7 @@
         <v>160</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C162" s="12"/>
       <c r="D162" s="11"/>
@@ -8004,7 +8072,7 @@
         <v>161</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C163" s="12"/>
       <c r="D163" s="11"/>
@@ -8018,7 +8086,7 @@
         <v>162</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C164" s="12"/>
       <c r="D164" s="11"/>
@@ -8032,7 +8100,7 @@
         <v>163</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C165" s="12"/>
       <c r="D165" s="11"/>
@@ -8046,7 +8114,7 @@
         <v>164</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C166" s="12"/>
       <c r="D166" s="11"/>
@@ -8060,7 +8128,7 @@
         <v>165</v>
       </c>
       <c r="B167" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C167" s="12"/>
       <c r="D167" s="11"/>
@@ -8074,7 +8142,7 @@
         <v>166</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C168" s="10"/>
       <c r="D168" s="11"/>
@@ -8088,7 +8156,7 @@
         <v>167</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C169" s="12"/>
       <c r="D169" s="11"/>
@@ -8102,7 +8170,7 @@
         <v>168</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C170" s="12"/>
       <c r="D170" s="11"/>
@@ -8116,7 +8184,7 @@
         <v>169</v>
       </c>
       <c r="B171" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C171" s="12"/>
       <c r="D171" s="11"/>
@@ -8130,7 +8198,7 @@
         <v>170</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C172" s="12"/>
       <c r="D172" s="11"/>
@@ -8144,7 +8212,7 @@
         <v>171</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C173" s="12"/>
       <c r="D173" s="11"/>
@@ -8158,7 +8226,7 @@
         <v>172</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C174" s="12"/>
       <c r="D174" s="11"/>
@@ -8172,7 +8240,7 @@
         <v>173</v>
       </c>
       <c r="B175" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C175" s="12"/>
       <c r="D175" s="11"/>
@@ -8186,7 +8254,7 @@
         <v>174</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C176" s="12"/>
       <c r="D176" s="11"/>
@@ -8200,7 +8268,7 @@
         <v>175</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C177" s="12"/>
       <c r="D177" s="11"/>
@@ -8214,7 +8282,7 @@
         <v>176</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C178" s="12"/>
       <c r="D178" s="11"/>
@@ -8228,7 +8296,7 @@
         <v>177</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C179" s="10"/>
       <c r="D179" s="11"/>
@@ -8242,7 +8310,7 @@
         <v>178</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C180" s="12"/>
       <c r="D180" s="11"/>
@@ -8256,7 +8324,7 @@
         <v>179</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C181" s="12"/>
       <c r="D181" s="11"/>
@@ -8270,7 +8338,7 @@
         <v>180</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C182" s="12"/>
       <c r="D182" s="11"/>
@@ -8284,7 +8352,7 @@
         <v>181</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C183" s="12"/>
       <c r="D183" s="11"/>
@@ -8298,7 +8366,7 @@
         <v>182</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C184" s="12"/>
       <c r="D184" s="11"/>
@@ -8312,7 +8380,7 @@
         <v>183</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C185" s="10"/>
       <c r="D185" s="11"/>
@@ -8326,7 +8394,7 @@
         <v>184</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C186" s="12"/>
       <c r="D186" s="11"/>
@@ -8340,7 +8408,7 @@
         <v>185</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C187" s="12"/>
       <c r="D187" s="11"/>
@@ -8354,7 +8422,7 @@
         <v>186</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C188" s="12"/>
       <c r="D188" s="11"/>
@@ -8368,7 +8436,7 @@
         <v>187</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C189" s="12"/>
       <c r="D189" s="11"/>
@@ -8382,7 +8450,7 @@
         <v>188</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C190" s="12"/>
       <c r="D190" s="11"/>
@@ -8396,7 +8464,7 @@
         <v>189</v>
       </c>
       <c r="B191" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C191" s="12"/>
       <c r="D191" s="11"/>
@@ -8410,7 +8478,7 @@
         <v>190</v>
       </c>
       <c r="B192" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C192" s="12"/>
       <c r="D192" s="11"/>
@@ -8424,7 +8492,7 @@
         <v>191</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C193" s="12"/>
       <c r="D193" s="11"/>
@@ -8438,7 +8506,7 @@
         <v>192</v>
       </c>
       <c r="B194" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C194" s="12"/>
       <c r="D194" s="11"/>
@@ -8452,7 +8520,7 @@
         <v>193</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C195" s="12"/>
       <c r="D195" s="11"/>
@@ -8466,7 +8534,7 @@
         <v>194</v>
       </c>
       <c r="B196" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C196" s="12"/>
       <c r="D196" s="11"/>
@@ -8480,7 +8548,7 @@
         <v>195</v>
       </c>
       <c r="B197" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C197" s="12"/>
       <c r="D197" s="11"/>
@@ -8494,7 +8562,7 @@
         <v>196</v>
       </c>
       <c r="B198" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C198" s="12"/>
       <c r="D198" s="11"/>
@@ -8508,7 +8576,7 @@
         <v>197</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C199" s="12"/>
       <c r="D199" s="11"/>
@@ -8522,7 +8590,7 @@
         <v>198</v>
       </c>
       <c r="B200" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C200" s="12"/>
       <c r="D200" s="11"/>
@@ -8536,7 +8604,7 @@
         <v>199</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C201" s="12"/>
       <c r="D201" s="11"/>
@@ -8550,7 +8618,7 @@
         <v>200</v>
       </c>
       <c r="B202" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C202" s="12"/>
       <c r="D202" s="11"/>
@@ -8564,7 +8632,7 @@
         <v>201</v>
       </c>
       <c r="B203" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C203" s="12"/>
       <c r="D203" s="11"/>
@@ -8578,7 +8646,7 @@
         <v>202</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C204" s="12"/>
       <c r="D204" s="11"/>
@@ -8592,7 +8660,7 @@
         <v>203</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C205" s="12"/>
       <c r="D205" s="11"/>
@@ -8606,7 +8674,7 @@
         <v>204</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C206" s="12"/>
       <c r="D206" s="11"/>
@@ -8620,7 +8688,7 @@
         <v>205</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C207" s="12"/>
       <c r="D207" s="11"/>
@@ -8634,7 +8702,7 @@
         <v>206</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C208" s="12"/>
       <c r="D208" s="11"/>
@@ -8648,7 +8716,7 @@
         <v>207</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C209" s="12"/>
       <c r="D209" s="11"/>
@@ -8662,7 +8730,7 @@
         <v>208</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C210" s="12"/>
       <c r="D210" s="11"/>
@@ -8676,7 +8744,7 @@
         <v>209</v>
       </c>
       <c r="B211" s="9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C211" s="10"/>
       <c r="D211" s="11"/>
@@ -8690,7 +8758,7 @@
         <v>210</v>
       </c>
       <c r="B212" s="9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C212" s="12"/>
       <c r="D212" s="11"/>
@@ -8704,7 +8772,7 @@
         <v>211</v>
       </c>
       <c r="B213" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C213" s="10"/>
       <c r="D213" s="11"/>
@@ -8718,7 +8786,7 @@
         <v>212</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C214" s="10"/>
       <c r="D214" s="11"/>
@@ -8732,7 +8800,7 @@
         <v>213</v>
       </c>
       <c r="B215" s="9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C215" s="12"/>
       <c r="D215" s="11"/>
@@ -8746,7 +8814,7 @@
         <v>214</v>
       </c>
       <c r="B216" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C216" s="12"/>
       <c r="D216" s="11"/>
@@ -8760,7 +8828,7 @@
         <v>215</v>
       </c>
       <c r="B217" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C217" s="12"/>
       <c r="D217" s="11"/>
@@ -8774,7 +8842,7 @@
         <v>216</v>
       </c>
       <c r="B218" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C218" s="12"/>
       <c r="D218" s="11"/>
@@ -8788,7 +8856,7 @@
         <v>217</v>
       </c>
       <c r="B219" s="9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C219" s="12"/>
       <c r="D219" s="11"/>
@@ -8802,7 +8870,7 @@
         <v>218</v>
       </c>
       <c r="B220" s="9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C220" s="12"/>
       <c r="D220" s="11"/>
@@ -8816,7 +8884,7 @@
         <v>219</v>
       </c>
       <c r="B221" s="9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C221" s="10"/>
       <c r="D221" s="11"/>
@@ -8830,7 +8898,7 @@
         <v>220</v>
       </c>
       <c r="B222" s="9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C222" s="12"/>
       <c r="D222" s="11"/>
@@ -8844,7 +8912,7 @@
         <v>221</v>
       </c>
       <c r="B223" s="9" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C223" s="12"/>
       <c r="D223" s="11"/>
@@ -8858,7 +8926,7 @@
         <v>222</v>
       </c>
       <c r="B224" s="9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C224" s="12"/>
       <c r="D224" s="11"/>
@@ -8872,7 +8940,7 @@
         <v>223</v>
       </c>
       <c r="B225" s="9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C225" s="12"/>
       <c r="D225" s="11"/>
@@ -8886,7 +8954,7 @@
         <v>224</v>
       </c>
       <c r="B226" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C226" s="12"/>
       <c r="D226" s="11"/>
@@ -8900,7 +8968,7 @@
         <v>225</v>
       </c>
       <c r="B227" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C227" s="12"/>
       <c r="D227" s="11"/>
@@ -8914,7 +8982,7 @@
         <v>226</v>
       </c>
       <c r="B228" s="9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C228" s="12"/>
       <c r="D228" s="11"/>
@@ -8928,7 +8996,7 @@
         <v>227</v>
       </c>
       <c r="B229" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C229" s="12"/>
       <c r="D229" s="11"/>
@@ -8942,7 +9010,7 @@
         <v>228</v>
       </c>
       <c r="B230" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C230" s="12"/>
       <c r="D230" s="11"/>
@@ -8956,7 +9024,7 @@
         <v>229</v>
       </c>
       <c r="B231" s="9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C231" s="12"/>
       <c r="D231" s="11"/>
@@ -8970,7 +9038,7 @@
         <v>230</v>
       </c>
       <c r="B232" s="9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C232" s="12"/>
       <c r="D232" s="11"/>
@@ -8984,7 +9052,7 @@
         <v>231</v>
       </c>
       <c r="B233" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C233" s="12"/>
       <c r="D233" s="11"/>
@@ -8998,7 +9066,7 @@
         <v>232</v>
       </c>
       <c r="B234" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C234" s="12"/>
       <c r="D234" s="11"/>
@@ -9012,7 +9080,7 @@
         <v>233</v>
       </c>
       <c r="B235" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C235" s="12"/>
       <c r="D235" s="11"/>
@@ -9026,7 +9094,7 @@
         <v>234</v>
       </c>
       <c r="B236" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C236" s="12"/>
       <c r="D236" s="11"/>
@@ -9040,7 +9108,7 @@
         <v>235</v>
       </c>
       <c r="B237" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C237" s="12"/>
       <c r="D237" s="11"/>
@@ -9054,7 +9122,7 @@
         <v>236</v>
       </c>
       <c r="B238" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C238" s="12"/>
       <c r="D238" s="11"/>
@@ -9068,7 +9136,7 @@
         <v>237</v>
       </c>
       <c r="B239" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C239" s="12"/>
       <c r="D239" s="11"/>
@@ -9082,7 +9150,7 @@
         <v>238</v>
       </c>
       <c r="B240" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C240" s="12"/>
       <c r="D240" s="11"/>
@@ -9096,7 +9164,7 @@
         <v>239</v>
       </c>
       <c r="B241" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C241" s="12"/>
       <c r="D241" s="11"/>
@@ -9110,7 +9178,7 @@
         <v>240</v>
       </c>
       <c r="B242" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C242" s="12"/>
       <c r="D242" s="11"/>
@@ -9124,7 +9192,7 @@
         <v>241</v>
       </c>
       <c r="B243" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C243" s="12"/>
       <c r="D243" s="11"/>
@@ -9138,7 +9206,7 @@
         <v>242</v>
       </c>
       <c r="B244" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C244" s="12"/>
       <c r="D244" s="11"/>
@@ -9152,7 +9220,7 @@
         <v>243</v>
       </c>
       <c r="B245" s="9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C245" s="12"/>
       <c r="D245" s="11"/>
@@ -9166,7 +9234,7 @@
         <v>244</v>
       </c>
       <c r="B246" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C246" s="12"/>
       <c r="D246" s="11"/>
@@ -9180,7 +9248,7 @@
         <v>245</v>
       </c>
       <c r="B247" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C247" s="12"/>
       <c r="D247" s="11"/>
@@ -9194,7 +9262,7 @@
         <v>246</v>
       </c>
       <c r="B248" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C248" s="12"/>
       <c r="D248" s="11"/>
@@ -9208,7 +9276,7 @@
         <v>247</v>
       </c>
       <c r="B249" s="9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C249" s="12"/>
       <c r="D249" s="11"/>
@@ -9222,7 +9290,7 @@
         <v>248</v>
       </c>
       <c r="B250" s="9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C250" s="12"/>
       <c r="D250" s="11"/>
@@ -9236,7 +9304,7 @@
         <v>249</v>
       </c>
       <c r="B251" s="9" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C251" s="12"/>
       <c r="D251" s="11"/>
@@ -9250,7 +9318,7 @@
         <v>250</v>
       </c>
       <c r="B252" s="9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C252" s="12"/>
       <c r="D252" s="11"/>
@@ -9264,7 +9332,7 @@
         <v>251</v>
       </c>
       <c r="B253" s="9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C253" s="12"/>
       <c r="D253" s="11"/>
@@ -9278,7 +9346,7 @@
         <v>252</v>
       </c>
       <c r="B254" s="9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C254" s="12"/>
       <c r="D254" s="11"/>
@@ -9292,7 +9360,7 @@
         <v>253</v>
       </c>
       <c r="B255" s="9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C255" s="12"/>
       <c r="D255" s="11"/>
@@ -9306,7 +9374,7 @@
         <v>254</v>
       </c>
       <c r="B256" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C256" s="12"/>
       <c r="D256" s="11"/>
@@ -9320,7 +9388,7 @@
         <v>255</v>
       </c>
       <c r="B257" s="9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C257" s="12"/>
       <c r="D257" s="11"/>
@@ -9334,7 +9402,7 @@
         <v>256</v>
       </c>
       <c r="B258" s="9" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C258" s="12"/>
       <c r="D258" s="11"/>
@@ -9348,7 +9416,7 @@
         <v>257</v>
       </c>
       <c r="B259" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C259" s="12"/>
       <c r="D259" s="11"/>
@@ -9362,7 +9430,7 @@
         <v>258</v>
       </c>
       <c r="B260" s="9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C260" s="12"/>
       <c r="D260" s="11"/>
@@ -9376,7 +9444,7 @@
         <v>259</v>
       </c>
       <c r="B261" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C261" s="10"/>
       <c r="D261" s="11"/>
@@ -9390,7 +9458,7 @@
         <v>260</v>
       </c>
       <c r="B262" s="9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C262" s="12"/>
       <c r="D262" s="11"/>
@@ -9404,7 +9472,7 @@
         <v>261</v>
       </c>
       <c r="B263" s="9" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C263" s="12"/>
       <c r="D263" s="11"/>
@@ -9418,7 +9486,7 @@
         <v>262</v>
       </c>
       <c r="B264" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C264" s="12"/>
       <c r="D264" s="11"/>
@@ -9432,7 +9500,7 @@
         <v>263</v>
       </c>
       <c r="B265" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C265" s="12"/>
       <c r="D265" s="11"/>
@@ -9446,7 +9514,7 @@
         <v>264</v>
       </c>
       <c r="B266" s="9" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C266" s="12"/>
       <c r="D266" s="11"/>
@@ -9460,7 +9528,7 @@
         <v>265</v>
       </c>
       <c r="B267" s="9" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C267" s="12"/>
       <c r="D267" s="11"/>
@@ -9474,7 +9542,7 @@
         <v>266</v>
       </c>
       <c r="B268" s="9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C268" s="10"/>
       <c r="D268" s="11"/>
@@ -9488,7 +9556,7 @@
         <v>267</v>
       </c>
       <c r="B269" s="9" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C269" s="12"/>
       <c r="D269" s="11"/>
@@ -9502,7 +9570,7 @@
         <v>268</v>
       </c>
       <c r="B270" s="9" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C270" s="12"/>
       <c r="D270" s="11"/>
@@ -9516,7 +9584,7 @@
         <v>269</v>
       </c>
       <c r="B271" s="9" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C271" s="10"/>
       <c r="D271" s="11"/>
@@ -9530,7 +9598,7 @@
         <v>270</v>
       </c>
       <c r="B272" s="9" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C272" s="12"/>
       <c r="D272" s="11"/>
@@ -9544,7 +9612,7 @@
         <v>271</v>
       </c>
       <c r="B273" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C273" s="12"/>
       <c r="D273" s="11"/>
@@ -9558,7 +9626,7 @@
         <v>272</v>
       </c>
       <c r="B274" s="9" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C274" s="12"/>
       <c r="D274" s="11"/>
@@ -9572,7 +9640,7 @@
         <v>273</v>
       </c>
       <c r="B275" s="9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C275" s="12"/>
       <c r="D275" s="11"/>
@@ -9586,7 +9654,7 @@
         <v>274</v>
       </c>
       <c r="B276" s="9" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C276" s="12"/>
       <c r="D276" s="11"/>
@@ -9600,7 +9668,7 @@
         <v>275</v>
       </c>
       <c r="B277" s="9" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C277" s="12"/>
       <c r="D277" s="11"/>
@@ -9614,7 +9682,7 @@
         <v>276</v>
       </c>
       <c r="B278" s="9" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C278" s="12"/>
       <c r="D278" s="11"/>
@@ -9628,7 +9696,7 @@
         <v>277</v>
       </c>
       <c r="B279" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C279" s="10"/>
       <c r="D279" s="11"/>
@@ -9642,7 +9710,7 @@
         <v>278</v>
       </c>
       <c r="B280" s="9" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C280" s="12"/>
       <c r="D280" s="11"/>
@@ -9656,7 +9724,7 @@
         <v>279</v>
       </c>
       <c r="B281" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C281" s="12"/>
       <c r="D281" s="11"/>
@@ -9670,7 +9738,7 @@
         <v>280</v>
       </c>
       <c r="B282" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C282" s="12"/>
       <c r="D282" s="11"/>
@@ -9684,7 +9752,7 @@
         <v>281</v>
       </c>
       <c r="B283" s="9" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C283" s="10"/>
       <c r="D283" s="11"/>
@@ -9698,7 +9766,7 @@
         <v>282</v>
       </c>
       <c r="B284" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C284" s="12"/>
       <c r="D284" s="11"/>
@@ -9712,7 +9780,7 @@
         <v>283</v>
       </c>
       <c r="B285" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C285" s="12"/>
       <c r="D285" s="11"/>
@@ -9726,7 +9794,7 @@
         <v>284</v>
       </c>
       <c r="B286" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C286" s="12"/>
       <c r="D286" s="11"/>
@@ -9740,7 +9808,7 @@
         <v>285</v>
       </c>
       <c r="B287" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C287" s="10"/>
       <c r="D287" s="11"/>
@@ -9754,7 +9822,7 @@
         <v>286</v>
       </c>
       <c r="B288" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C288" s="12"/>
       <c r="D288" s="11"/>
@@ -9768,7 +9836,7 @@
         <v>287</v>
       </c>
       <c r="B289" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C289" s="12"/>
       <c r="D289" s="11"/>
@@ -9782,7 +9850,7 @@
         <v>288</v>
       </c>
       <c r="B290" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C290" s="12"/>
       <c r="D290" s="11"/>
@@ -9796,7 +9864,7 @@
         <v>289</v>
       </c>
       <c r="B291" s="9" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C291" s="12"/>
       <c r="D291" s="11"/>
@@ -9810,7 +9878,7 @@
         <v>290</v>
       </c>
       <c r="B292" s="9" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C292" s="12"/>
       <c r="D292" s="11"/>
@@ -9824,7 +9892,7 @@
         <v>291</v>
       </c>
       <c r="B293" s="9" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C293" s="12"/>
       <c r="D293" s="11"/>
@@ -9838,7 +9906,7 @@
         <v>292</v>
       </c>
       <c r="B294" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C294" s="12"/>
       <c r="D294" s="11"/>
@@ -9852,7 +9920,7 @@
         <v>293</v>
       </c>
       <c r="B295" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C295" s="10"/>
       <c r="D295" s="11"/>
@@ -9866,7 +9934,7 @@
         <v>294</v>
       </c>
       <c r="B296" s="9" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C296" s="12"/>
       <c r="D296" s="11"/>
@@ -9880,7 +9948,7 @@
         <v>295</v>
       </c>
       <c r="B297" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C297" s="12"/>
       <c r="D297" s="11"/>
@@ -9894,7 +9962,7 @@
         <v>296</v>
       </c>
       <c r="B298" s="9" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C298" s="12"/>
       <c r="D298" s="11"/>
@@ -9908,7 +9976,7 @@
         <v>297</v>
       </c>
       <c r="B299" s="9" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C299" s="12"/>
       <c r="D299" s="11"/>
@@ -9922,7 +9990,7 @@
         <v>298</v>
       </c>
       <c r="B300" s="9" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C300" s="12"/>
       <c r="D300" s="11"/>
@@ -9936,7 +10004,7 @@
         <v>299</v>
       </c>
       <c r="B301" s="9" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C301" s="12"/>
       <c r="D301" s="11"/>
@@ -9950,7 +10018,7 @@
         <v>300</v>
       </c>
       <c r="B302" s="9" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C302" s="12"/>
       <c r="D302" s="11"/>
@@ -9964,7 +10032,7 @@
         <v>301</v>
       </c>
       <c r="B303" s="9" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C303" s="12"/>
       <c r="D303" s="11"/>
@@ -9978,7 +10046,7 @@
         <v>302</v>
       </c>
       <c r="B304" s="9" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C304" s="12"/>
       <c r="D304" s="11"/>
@@ -9992,7 +10060,7 @@
         <v>303</v>
       </c>
       <c r="B305" s="9" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C305" s="12"/>
       <c r="D305" s="11"/>
@@ -10006,7 +10074,7 @@
         <v>304</v>
       </c>
       <c r="B306" s="9" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C306" s="12"/>
       <c r="D306" s="11"/>
@@ -10020,7 +10088,7 @@
         <v>305</v>
       </c>
       <c r="B307" s="9" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C307" s="12"/>
       <c r="D307" s="11"/>
@@ -10034,7 +10102,7 @@
         <v>306</v>
       </c>
       <c r="B308" s="9" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C308" s="12"/>
       <c r="D308" s="11"/>
@@ -10048,7 +10116,7 @@
         <v>307</v>
       </c>
       <c r="B309" s="9" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C309" s="12"/>
       <c r="D309" s="11"/>
@@ -10062,7 +10130,7 @@
         <v>308</v>
       </c>
       <c r="B310" s="9" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C310" s="12"/>
       <c r="D310" s="11"/>
@@ -10076,7 +10144,7 @@
         <v>309</v>
       </c>
       <c r="B311" s="9" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C311" s="12"/>
       <c r="D311" s="11"/>
@@ -10090,7 +10158,7 @@
         <v>310</v>
       </c>
       <c r="B312" s="9" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C312" s="12"/>
       <c r="D312" s="11"/>
@@ -10104,7 +10172,7 @@
         <v>311</v>
       </c>
       <c r="B313" s="9" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C313" s="12"/>
       <c r="D313" s="11"/>
@@ -10118,7 +10186,7 @@
         <v>312</v>
       </c>
       <c r="B314" s="9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C314" s="12"/>
       <c r="D314" s="11"/>
@@ -10132,7 +10200,7 @@
         <v>313</v>
       </c>
       <c r="B315" s="9" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C315" s="12"/>
       <c r="D315" s="11"/>
@@ -10146,7 +10214,7 @@
         <v>314</v>
       </c>
       <c r="B316" s="9" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C316" s="12"/>
       <c r="D316" s="11"/>
@@ -10160,7 +10228,7 @@
         <v>315</v>
       </c>
       <c r="B317" s="9" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C317" s="12"/>
       <c r="D317" s="11"/>
@@ -10174,7 +10242,7 @@
         <v>316</v>
       </c>
       <c r="B318" s="9" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C318" s="12"/>
       <c r="D318" s="11"/>
@@ -10188,7 +10256,7 @@
         <v>317</v>
       </c>
       <c r="B319" s="9" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C319" s="12"/>
       <c r="D319" s="11"/>
@@ -10202,7 +10270,7 @@
         <v>318</v>
       </c>
       <c r="B320" s="9" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C320" s="12"/>
       <c r="D320" s="11"/>
@@ -10216,7 +10284,7 @@
         <v>319</v>
       </c>
       <c r="B321" s="9" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C321" s="12"/>
       <c r="D321" s="11"/>
@@ -10230,7 +10298,7 @@
         <v>320</v>
       </c>
       <c r="B322" s="9" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C322" s="10"/>
       <c r="D322" s="11"/>
@@ -10244,7 +10312,7 @@
         <v>321</v>
       </c>
       <c r="B323" s="9" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C323" s="12"/>
       <c r="D323" s="11"/>
@@ -10258,7 +10326,7 @@
         <v>322</v>
       </c>
       <c r="B324" s="9" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C324" s="12"/>
       <c r="D324" s="11"/>
@@ -10272,7 +10340,7 @@
         <v>323</v>
       </c>
       <c r="B325" s="9" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C325" s="12"/>
       <c r="D325" s="11"/>
@@ -10286,7 +10354,7 @@
         <v>324</v>
       </c>
       <c r="B326" s="9" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C326" s="12"/>
       <c r="D326" s="11"/>
@@ -10300,7 +10368,7 @@
         <v>325</v>
       </c>
       <c r="B327" s="9" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C327" s="12"/>
       <c r="D327" s="11"/>
@@ -10314,7 +10382,7 @@
         <v>326</v>
       </c>
       <c r="B328" s="9" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C328" s="12"/>
       <c r="D328" s="11"/>
@@ -10328,7 +10396,7 @@
         <v>327</v>
       </c>
       <c r="B329" s="9" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C329" s="12"/>
       <c r="D329" s="11"/>
@@ -10342,7 +10410,7 @@
         <v>328</v>
       </c>
       <c r="B330" s="9" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C330" s="12"/>
       <c r="D330" s="11"/>
@@ -10356,7 +10424,7 @@
         <v>329</v>
       </c>
       <c r="B331" s="9" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C331" s="12"/>
       <c r="D331" s="11"/>
@@ -10370,7 +10438,7 @@
         <v>330</v>
       </c>
       <c r="B332" s="9" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C332" s="12"/>
       <c r="D332" s="11"/>
@@ -10384,7 +10452,7 @@
         <v>331</v>
       </c>
       <c r="B333" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C333" s="12"/>
       <c r="D333" s="11"/>
@@ -10398,7 +10466,7 @@
         <v>332</v>
       </c>
       <c r="B334" s="9" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C334" s="12"/>
       <c r="D334" s="11"/>
@@ -10412,7 +10480,7 @@
         <v>333</v>
       </c>
       <c r="B335" s="9" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C335" s="12"/>
       <c r="D335" s="11"/>

</xml_diff>

<commit_message>
RQ2 250 manual analysis
</commit_message>
<xml_diff>
--- a/RQ2_Commit_Manual_Analysis_Tejas.xlsx
+++ b/RQ2_Commit_Manual_Analysis_Tejas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Thesis\CPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tejasvaity/Documents/thesis/cps/cps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69517D9-6A98-4C00-BE26-E19619C207CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6E8BA0-6585-8148-9BAF-7969016C11B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17180" yWindow="940" windowWidth="16860" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="525">
   <si>
     <t>Table 1</t>
   </si>
@@ -4085,13 +4085,214 @@
   </si>
   <si>
     <t>added environment variables, install linux-x86_64</t>
+  </si>
+  <si>
+    <t>create a directory and change its permsission, add the environment variable.</t>
+  </si>
+  <si>
+    <t>changed the version of tar file</t>
+  </si>
+  <si>
+    <t>bulding the image for AVR32</t>
+  </si>
+  <si>
+    <t>interchange the step by step build</t>
+  </si>
+  <si>
+    <t>removing files creating space for the memory</t>
+  </si>
+  <si>
+    <t>using different image</t>
+  </si>
+  <si>
+    <t>chnaged tag from default to linux and amd64</t>
+  </si>
+  <si>
+    <t>added command to run docker_build</t>
+  </si>
+  <si>
+    <t>changed the version of image + added services in .yml files</t>
+  </si>
+  <si>
+    <t>formatting removing spaces.</t>
+  </si>
+  <si>
+    <t>install python serial</t>
+  </si>
+  <si>
+    <t>removing the log files</t>
+  </si>
+  <si>
+    <t>add a pre built image</t>
+  </si>
+  <si>
+    <t>removed the starting point of application.</t>
+  </si>
+  <si>
+    <t>in .yaml add tensor library</t>
+  </si>
+  <si>
+    <t>in .yaml changed tag-suffix</t>
+  </si>
+  <si>
+    <t>in .yaml use different files</t>
+  </si>
+  <si>
+    <t>copy files to different location.</t>
+  </si>
+  <si>
+    <t>created and modifies new .yaml files for the github actions</t>
+  </si>
+  <si>
+    <t>added picture and changes in readme file.</t>
+  </si>
+  <si>
+    <t>added tag in .yaml</t>
+  </si>
+  <si>
+    <t>copy and run source files</t>
+  </si>
+  <si>
+    <t>copy and run source files. Run the script and image</t>
+  </si>
+  <si>
+    <t>created a new script for cleaning up the system files and replaced them in dockerfile.</t>
+  </si>
+  <si>
+    <t>added a command to update</t>
+  </si>
+  <si>
+    <t>changed the version of image + install and remove older builds.</t>
+  </si>
+  <si>
+    <t>install virtual environment</t>
+  </si>
+  <si>
+    <t>install python dependencies</t>
+  </si>
+  <si>
+    <t>added a comment + remove command to run bazel</t>
+  </si>
+  <si>
+    <t>deleted the dockerfile</t>
+  </si>
+  <si>
+    <t>add installing build command + remove old builds and install, run new builds</t>
+  </si>
+  <si>
+    <t>remove softlinks and create new environment variables.</t>
+  </si>
+  <si>
+    <t>fix the spelling error.</t>
+  </si>
+  <si>
+    <t>modified the github actions files.</t>
+  </si>
+  <si>
+    <t>chnages in github actions files and in dockerUtilities.ts file chnages in method argument.</t>
+  </si>
+  <si>
+    <t>run and install new dependencies and build</t>
+  </si>
+  <si>
+    <t>Adding user agent as "Mozilla" to trick the server into thinking the request is coming from a web browser.</t>
+  </si>
+  <si>
+    <t>install libraries</t>
+  </si>
+  <si>
+    <t>change in version of libraries.</t>
+  </si>
+  <si>
+    <t>spelling mistake in print statement.</t>
+  </si>
+  <si>
+    <t>remove a library</t>
+  </si>
+  <si>
+    <t>change the script</t>
+  </si>
+  <si>
+    <t>install single libraby removed other library and run script without argument.</t>
+  </si>
+  <si>
+    <t>create environment variables</t>
+  </si>
+  <si>
+    <t>run different script.</t>
+  </si>
+  <si>
+    <t>Adds support for --quiet mode in Docker builds so that output is reduced to only errors and also there is no progress stream.</t>
+  </si>
+  <si>
+    <t>no change.</t>
+  </si>
+  <si>
+    <t>add structure datatype. Add function for cleanup and output.</t>
+  </si>
+  <si>
+    <t>removed the print statement.</t>
+  </si>
+  <si>
+    <t>changed the logic for pre pull cache images.</t>
+  </si>
+  <si>
+    <t>modify the structure datatype. Add condition for Auto Label.</t>
+  </si>
+  <si>
+    <t>changed the sequence of import library.</t>
+  </si>
+  <si>
+    <t>change the file location.</t>
+  </si>
+  <si>
+    <t>changed the version of image + downloading and running that image.</t>
+  </si>
+  <si>
+    <t>removing the platform specific images to default image which can run on all the machine.</t>
+  </si>
+  <si>
+    <t>changes in tar file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changes in tar file and update chart </t>
+  </si>
+  <si>
+    <t>install dependencies and run as user</t>
+  </si>
+  <si>
+    <t>change the directory and run python code</t>
+  </si>
+  <si>
+    <t>add specific version of tourch library</t>
+  </si>
+  <si>
+    <t>set the path for python and carla. Chnages in script for adding different tag name for docker image.</t>
+  </si>
+  <si>
+    <t>install dependencies and set environment variables.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chnaged the script to get input argument and now update the build. </t>
+  </si>
+  <si>
+    <t>changed the python version and renamed tar file.</t>
+  </si>
+  <si>
+    <t>add a dataset and run python server.</t>
+  </si>
+  <si>
+    <t>install Cuda from different git repo</t>
+  </si>
+  <si>
+    <t>added a new script file and changed the port no. in script.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -4120,6 +4321,12 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -4307,7 +4514,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4358,6 +4565,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5492,11 +5708,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H335"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B140" workbookViewId="0">
-      <selection activeCell="B151" sqref="B151"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A243" zoomScale="111" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C252" sqref="C252"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="88.33203125" style="1" customWidth="1"/>
@@ -5505,7 +5721,7 @@
     <col min="10" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.6" customHeight="1">
+    <row r="1" spans="1:8" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -5517,7 +5733,7 @@
       <c r="G1" s="15"/>
       <c r="H1" s="16"/>
     </row>
-    <row r="2" spans="1:8" ht="20.25" customHeight="1">
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5533,7 +5749,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="20.25" customHeight="1">
+    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -5549,7 +5765,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -5565,7 +5781,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -5581,7 +5797,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" ht="32.1" customHeight="1">
+    <row r="6" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -5597,7 +5813,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:8" ht="32.1" customHeight="1">
+    <row r="7" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -5613,7 +5829,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8" ht="32.1" customHeight="1">
+    <row r="8" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -5629,7 +5845,7 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -5645,7 +5861,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8" ht="44.1" customHeight="1">
+    <row r="10" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -5661,7 +5877,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="1:8" ht="32.1" customHeight="1">
+    <row r="11" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -5677,7 +5893,7 @@
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="1:8" ht="32.1" customHeight="1">
+    <row r="12" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -5693,7 +5909,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:8" ht="32.1" customHeight="1">
+    <row r="13" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -5709,7 +5925,7 @@
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="1:8" ht="32.1" customHeight="1">
+    <row r="14" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -5725,7 +5941,7 @@
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:8" ht="44.1" customHeight="1">
+    <row r="15" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -5741,7 +5957,7 @@
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
-    <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -5757,7 +5973,7 @@
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
     </row>
-    <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -5773,7 +5989,7 @@
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
     </row>
-    <row r="18" spans="1:8" ht="56.1" customHeight="1">
+    <row r="18" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="8">
         <v>16</v>
       </c>
@@ -5789,7 +6005,7 @@
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
     </row>
-    <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="8">
         <v>17</v>
       </c>
@@ -5805,7 +6021,7 @@
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
     </row>
-    <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="8">
         <v>18</v>
       </c>
@@ -5821,7 +6037,7 @@
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
     </row>
-    <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="8">
         <v>19</v>
       </c>
@@ -5837,7 +6053,7 @@
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="1:8" ht="56.1" customHeight="1">
+    <row r="22" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="8">
         <v>20</v>
       </c>
@@ -5853,7 +6069,7 @@
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
     </row>
-    <row r="23" spans="1:8" ht="68.099999999999994" customHeight="1">
+    <row r="23" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="8">
         <v>21</v>
       </c>
@@ -5869,7 +6085,7 @@
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
     </row>
-    <row r="24" spans="1:8" ht="56.1" customHeight="1">
+    <row r="24" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="8">
         <v>22</v>
       </c>
@@ -5885,7 +6101,7 @@
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="1:8" ht="44.1" customHeight="1">
+    <row r="25" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="8">
         <v>23</v>
       </c>
@@ -5901,7 +6117,7 @@
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
     </row>
-    <row r="26" spans="1:8" ht="32.1" customHeight="1">
+    <row r="26" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="8">
         <v>24</v>
       </c>
@@ -5917,7 +6133,7 @@
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
     </row>
-    <row r="27" spans="1:8" ht="32.1" customHeight="1">
+    <row r="27" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="8">
         <v>25</v>
       </c>
@@ -5933,7 +6149,7 @@
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
     </row>
-    <row r="28" spans="1:8" ht="32.1" customHeight="1">
+    <row r="28" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="8">
         <v>26</v>
       </c>
@@ -5949,7 +6165,7 @@
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
     </row>
-    <row r="29" spans="1:8" ht="44.1" customHeight="1">
+    <row r="29" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="8">
         <v>27</v>
       </c>
@@ -5965,7 +6181,7 @@
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
     </row>
-    <row r="30" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="8">
         <v>28</v>
       </c>
@@ -5981,7 +6197,7 @@
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
     </row>
-    <row r="31" spans="1:8" ht="56.1" customHeight="1">
+    <row r="31" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="8">
         <v>29</v>
       </c>
@@ -5997,7 +6213,7 @@
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
     </row>
-    <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="8">
         <v>30</v>
       </c>
@@ -6013,7 +6229,7 @@
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
     </row>
-    <row r="33" spans="1:8" ht="32.1" customHeight="1">
+    <row r="33" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="8">
         <v>31</v>
       </c>
@@ -6029,7 +6245,7 @@
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
     </row>
-    <row r="34" spans="1:8" ht="32.1" customHeight="1">
+    <row r="34" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="8">
         <v>32</v>
       </c>
@@ -6045,7 +6261,7 @@
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
     </row>
-    <row r="35" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="35" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="8">
         <v>33</v>
       </c>
@@ -6059,7 +6275,7 @@
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
     </row>
-    <row r="36" spans="1:8" ht="44.1" customHeight="1">
+    <row r="36" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="8">
         <v>34</v>
       </c>
@@ -6075,7 +6291,7 @@
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
     </row>
-    <row r="37" spans="1:8" ht="32.1" customHeight="1">
+    <row r="37" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="8">
         <v>35</v>
       </c>
@@ -6091,7 +6307,7 @@
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
     </row>
-    <row r="38" spans="1:8" ht="44.1" customHeight="1">
+    <row r="38" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="8">
         <v>36</v>
       </c>
@@ -6107,7 +6323,7 @@
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
     </row>
-    <row r="39" spans="1:8" ht="56.1" customHeight="1">
+    <row r="39" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="8">
         <v>37</v>
       </c>
@@ -6123,7 +6339,7 @@
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
     </row>
-    <row r="40" spans="1:8" ht="44.1" customHeight="1">
+    <row r="40" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="8">
         <v>38</v>
       </c>
@@ -6139,7 +6355,7 @@
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
     </row>
-    <row r="41" spans="1:8" ht="44.1" customHeight="1">
+    <row r="41" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="8">
         <v>39</v>
       </c>
@@ -6155,7 +6371,7 @@
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
     </row>
-    <row r="42" spans="1:8" ht="56.1" customHeight="1">
+    <row r="42" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="8">
         <v>40</v>
       </c>
@@ -6171,7 +6387,7 @@
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
     </row>
-    <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="43" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="8">
         <v>41</v>
       </c>
@@ -6187,7 +6403,7 @@
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
     </row>
-    <row r="44" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="44" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="8">
         <v>42</v>
       </c>
@@ -6203,7 +6419,7 @@
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
     </row>
-    <row r="45" spans="1:8" ht="68.099999999999994" customHeight="1">
+    <row r="45" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="8">
         <v>43</v>
       </c>
@@ -6219,7 +6435,7 @@
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
     </row>
-    <row r="46" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="46" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="8">
         <v>44</v>
       </c>
@@ -6235,7 +6451,7 @@
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
     </row>
-    <row r="47" spans="1:8" ht="32.1" customHeight="1">
+    <row r="47" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="8">
         <v>45</v>
       </c>
@@ -6251,7 +6467,7 @@
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
     </row>
-    <row r="48" spans="1:8" ht="44.1" customHeight="1">
+    <row r="48" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="8">
         <v>46</v>
       </c>
@@ -6267,7 +6483,7 @@
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
     </row>
-    <row r="49" spans="1:8" ht="32.1" customHeight="1">
+    <row r="49" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="8">
         <v>47</v>
       </c>
@@ -6283,7 +6499,7 @@
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
     </row>
-    <row r="50" spans="1:8" ht="32.1" customHeight="1">
+    <row r="50" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="8">
         <v>48</v>
       </c>
@@ -6299,7 +6515,7 @@
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
     </row>
-    <row r="51" spans="1:8" ht="44.1" customHeight="1">
+    <row r="51" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="8">
         <v>49</v>
       </c>
@@ -6315,7 +6531,7 @@
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
     </row>
-    <row r="52" spans="1:8" ht="44.1" customHeight="1">
+    <row r="52" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="8">
         <v>50</v>
       </c>
@@ -6331,7 +6547,7 @@
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
     </row>
-    <row r="53" spans="1:8" ht="32.1" customHeight="1">
+    <row r="53" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="8">
         <v>51</v>
       </c>
@@ -6347,7 +6563,7 @@
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
     </row>
-    <row r="54" spans="1:8" ht="32.1" customHeight="1">
+    <row r="54" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="8">
         <v>52</v>
       </c>
@@ -6363,7 +6579,7 @@
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
     </row>
-    <row r="55" spans="1:8" ht="32.1" customHeight="1">
+    <row r="55" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="8">
         <v>53</v>
       </c>
@@ -6379,7 +6595,7 @@
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
     </row>
-    <row r="56" spans="1:8" ht="32.1" customHeight="1">
+    <row r="56" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="8">
         <v>54</v>
       </c>
@@ -6395,7 +6611,7 @@
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
     </row>
-    <row r="57" spans="1:8" ht="44.1" customHeight="1">
+    <row r="57" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="8">
         <v>55</v>
       </c>
@@ -6411,7 +6627,7 @@
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
     </row>
-    <row r="58" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="58" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="8">
         <v>56</v>
       </c>
@@ -6427,7 +6643,7 @@
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
     </row>
-    <row r="59" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="59" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="8">
         <v>57</v>
       </c>
@@ -6443,7 +6659,7 @@
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
     </row>
-    <row r="60" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="60" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="8">
         <v>58</v>
       </c>
@@ -6459,7 +6675,7 @@
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
     </row>
-    <row r="61" spans="1:8" ht="44.1" customHeight="1">
+    <row r="61" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="8">
         <v>59</v>
       </c>
@@ -6475,7 +6691,7 @@
       <c r="G61" s="11"/>
       <c r="H61" s="11"/>
     </row>
-    <row r="62" spans="1:8" ht="32.1" customHeight="1">
+    <row r="62" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="8">
         <v>60</v>
       </c>
@@ -6491,7 +6707,7 @@
       <c r="G62" s="11"/>
       <c r="H62" s="11"/>
     </row>
-    <row r="63" spans="1:8" ht="44.1" customHeight="1">
+    <row r="63" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="8">
         <v>61</v>
       </c>
@@ -6507,7 +6723,7 @@
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
     </row>
-    <row r="64" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="64" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="8">
         <v>62</v>
       </c>
@@ -6523,7 +6739,7 @@
       <c r="G64" s="11"/>
       <c r="H64" s="11"/>
     </row>
-    <row r="65" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="65" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="8">
         <v>63</v>
       </c>
@@ -6539,7 +6755,7 @@
       <c r="G65" s="11"/>
       <c r="H65" s="11"/>
     </row>
-    <row r="66" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="66" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="8">
         <v>64</v>
       </c>
@@ -6555,7 +6771,7 @@
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
     </row>
-    <row r="67" spans="1:8" ht="32.1" customHeight="1">
+    <row r="67" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="8">
         <v>65</v>
       </c>
@@ -6571,7 +6787,7 @@
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
     </row>
-    <row r="68" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="68" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="8">
         <v>66</v>
       </c>
@@ -6587,7 +6803,7 @@
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
     </row>
-    <row r="69" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="69" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="8">
         <v>67</v>
       </c>
@@ -6603,7 +6819,7 @@
       <c r="G69" s="11"/>
       <c r="H69" s="11"/>
     </row>
-    <row r="70" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="70" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="8">
         <v>68</v>
       </c>
@@ -6619,7 +6835,7 @@
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
     </row>
-    <row r="71" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="71" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="8">
         <v>69</v>
       </c>
@@ -6635,7 +6851,7 @@
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
     </row>
-    <row r="72" spans="1:8" ht="32.1" customHeight="1">
+    <row r="72" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="8">
         <v>70</v>
       </c>
@@ -6651,7 +6867,7 @@
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
     </row>
-    <row r="73" spans="1:8" ht="32.1" customHeight="1">
+    <row r="73" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="8">
         <v>71</v>
       </c>
@@ -6667,7 +6883,7 @@
       <c r="G73" s="11"/>
       <c r="H73" s="11"/>
     </row>
-    <row r="74" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="74" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="8">
         <v>72</v>
       </c>
@@ -6683,7 +6899,7 @@
       <c r="G74" s="11"/>
       <c r="H74" s="11"/>
     </row>
-    <row r="75" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="75" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="8">
         <v>73</v>
       </c>
@@ -6699,7 +6915,7 @@
       <c r="G75" s="11"/>
       <c r="H75" s="11"/>
     </row>
-    <row r="76" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="76" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="8">
         <v>74</v>
       </c>
@@ -6715,7 +6931,7 @@
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
     </row>
-    <row r="77" spans="1:8" ht="32.1" customHeight="1">
+    <row r="77" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="8">
         <v>75</v>
       </c>
@@ -6731,7 +6947,7 @@
       <c r="G77" s="11"/>
       <c r="H77" s="11"/>
     </row>
-    <row r="78" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="78" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="8">
         <v>76</v>
       </c>
@@ -6747,7 +6963,7 @@
       <c r="G78" s="11"/>
       <c r="H78" s="11"/>
     </row>
-    <row r="79" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="79" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="8">
         <v>77</v>
       </c>
@@ -6763,7 +6979,7 @@
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
     </row>
-    <row r="80" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="80" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="8">
         <v>78</v>
       </c>
@@ -6779,7 +6995,7 @@
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
     </row>
-    <row r="81" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="81" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="8">
         <v>79</v>
       </c>
@@ -6795,7 +7011,7 @@
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
     </row>
-    <row r="82" spans="1:8" ht="68.099999999999994" customHeight="1">
+    <row r="82" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="8">
         <v>80</v>
       </c>
@@ -6811,7 +7027,7 @@
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
     </row>
-    <row r="83" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="83" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="8">
         <v>81</v>
       </c>
@@ -6827,7 +7043,7 @@
       <c r="G83" s="11"/>
       <c r="H83" s="11"/>
     </row>
-    <row r="84" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="84" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="8">
         <v>82</v>
       </c>
@@ -6843,7 +7059,7 @@
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
     </row>
-    <row r="85" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="85" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="8">
         <v>83</v>
       </c>
@@ -6859,7 +7075,7 @@
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
     </row>
-    <row r="86" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="86" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="8">
         <v>84</v>
       </c>
@@ -6875,7 +7091,7 @@
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
     </row>
-    <row r="87" spans="1:8" ht="32.1" customHeight="1">
+    <row r="87" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="8">
         <v>85</v>
       </c>
@@ -6891,7 +7107,7 @@
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
     </row>
-    <row r="88" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="88" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="8">
         <v>86</v>
       </c>
@@ -6907,7 +7123,7 @@
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
     </row>
-    <row r="89" spans="1:8" ht="32.1" customHeight="1">
+    <row r="89" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="8">
         <v>87</v>
       </c>
@@ -6923,7 +7139,7 @@
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
     </row>
-    <row r="90" spans="1:8" ht="68.099999999999994" customHeight="1">
+    <row r="90" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="8">
         <v>88</v>
       </c>
@@ -6939,7 +7155,7 @@
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
     </row>
-    <row r="91" spans="1:8" ht="32.1" customHeight="1">
+    <row r="91" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="8">
         <v>89</v>
       </c>
@@ -6955,7 +7171,7 @@
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
     </row>
-    <row r="92" spans="1:8" ht="32.1" customHeight="1">
+    <row r="92" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="8">
         <v>90</v>
       </c>
@@ -6971,7 +7187,7 @@
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
     </row>
-    <row r="93" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="93" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="8">
         <v>91</v>
       </c>
@@ -6987,7 +7203,7 @@
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
     </row>
-    <row r="94" spans="1:8" ht="56.1" customHeight="1">
+    <row r="94" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="8">
         <v>92</v>
       </c>
@@ -7003,7 +7219,7 @@
       <c r="G94" s="11"/>
       <c r="H94" s="11"/>
     </row>
-    <row r="95" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="95" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="8">
         <v>93</v>
       </c>
@@ -7019,7 +7235,7 @@
       <c r="G95" s="11"/>
       <c r="H95" s="11"/>
     </row>
-    <row r="96" spans="1:8" ht="32.1" customHeight="1">
+    <row r="96" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="8">
         <v>94</v>
       </c>
@@ -7035,7 +7251,7 @@
       <c r="G96" s="11"/>
       <c r="H96" s="11"/>
     </row>
-    <row r="97" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="97" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="8">
         <v>95</v>
       </c>
@@ -7051,7 +7267,7 @@
       <c r="G97" s="11"/>
       <c r="H97" s="11"/>
     </row>
-    <row r="98" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="98" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="8">
         <v>96</v>
       </c>
@@ -7067,7 +7283,7 @@
       <c r="G98" s="11"/>
       <c r="H98" s="11"/>
     </row>
-    <row r="99" spans="1:8" ht="32.1" customHeight="1">
+    <row r="99" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="8">
         <v>97</v>
       </c>
@@ -7083,7 +7299,7 @@
       <c r="G99" s="11"/>
       <c r="H99" s="11"/>
     </row>
-    <row r="100" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="100" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="8">
         <v>98</v>
       </c>
@@ -7099,7 +7315,7 @@
       <c r="G100" s="11"/>
       <c r="H100" s="11"/>
     </row>
-    <row r="101" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="101" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="8">
         <v>99</v>
       </c>
@@ -7115,7 +7331,7 @@
       <c r="G101" s="11"/>
       <c r="H101" s="11"/>
     </row>
-    <row r="102" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="102" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="8">
         <v>100</v>
       </c>
@@ -7131,7 +7347,7 @@
       <c r="G102" s="11"/>
       <c r="H102" s="11"/>
     </row>
-    <row r="103" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="103" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="8">
         <v>101</v>
       </c>
@@ -7147,7 +7363,7 @@
       <c r="G103" s="11"/>
       <c r="H103" s="11"/>
     </row>
-    <row r="104" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="104" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="8">
         <v>102</v>
       </c>
@@ -7163,7 +7379,7 @@
       <c r="G104" s="11"/>
       <c r="H104" s="11"/>
     </row>
-    <row r="105" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="105" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="8">
         <v>103</v>
       </c>
@@ -7179,7 +7395,7 @@
       <c r="G105" s="11"/>
       <c r="H105" s="11"/>
     </row>
-    <row r="106" spans="1:8" ht="32.1" customHeight="1">
+    <row r="106" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="8">
         <v>104</v>
       </c>
@@ -7195,7 +7411,7 @@
       <c r="G106" s="11"/>
       <c r="H106" s="11"/>
     </row>
-    <row r="107" spans="1:8" ht="44.1" customHeight="1">
+    <row r="107" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="8">
         <v>105</v>
       </c>
@@ -7211,7 +7427,7 @@
       <c r="G107" s="11"/>
       <c r="H107" s="11"/>
     </row>
-    <row r="108" spans="1:8" ht="32.1" customHeight="1">
+    <row r="108" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="8">
         <v>106</v>
       </c>
@@ -7227,7 +7443,7 @@
       <c r="G108" s="11"/>
       <c r="H108" s="11"/>
     </row>
-    <row r="109" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="109" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="8">
         <v>107</v>
       </c>
@@ -7243,7 +7459,7 @@
       <c r="G109" s="11"/>
       <c r="H109" s="11"/>
     </row>
-    <row r="110" spans="1:8" ht="32.1" customHeight="1">
+    <row r="110" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="8">
         <v>108</v>
       </c>
@@ -7259,7 +7475,7 @@
       <c r="G110" s="11"/>
       <c r="H110" s="11"/>
     </row>
-    <row r="111" spans="1:8" ht="32.1" customHeight="1">
+    <row r="111" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="8">
         <v>109</v>
       </c>
@@ -7275,7 +7491,7 @@
       <c r="G111" s="11"/>
       <c r="H111" s="11"/>
     </row>
-    <row r="112" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="112" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="8">
         <v>110</v>
       </c>
@@ -7291,7 +7507,7 @@
       <c r="G112" s="11"/>
       <c r="H112" s="11"/>
     </row>
-    <row r="113" spans="1:8" ht="32.1" customHeight="1">
+    <row r="113" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="8">
         <v>111</v>
       </c>
@@ -7307,7 +7523,7 @@
       <c r="G113" s="11"/>
       <c r="H113" s="11"/>
     </row>
-    <row r="114" spans="1:8" ht="32.1" customHeight="1">
+    <row r="114" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="8">
         <v>112</v>
       </c>
@@ -7323,7 +7539,7 @@
       <c r="G114" s="11"/>
       <c r="H114" s="11"/>
     </row>
-    <row r="115" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="115" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="8">
         <v>113</v>
       </c>
@@ -7339,7 +7555,7 @@
       <c r="G115" s="11"/>
       <c r="H115" s="11"/>
     </row>
-    <row r="116" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="116" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="8">
         <v>114</v>
       </c>
@@ -7355,7 +7571,7 @@
       <c r="G116" s="11"/>
       <c r="H116" s="11"/>
     </row>
-    <row r="117" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="117" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="8">
         <v>115</v>
       </c>
@@ -7371,7 +7587,7 @@
       <c r="G117" s="11"/>
       <c r="H117" s="11"/>
     </row>
-    <row r="118" spans="1:8" ht="32.1" customHeight="1">
+    <row r="118" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118" s="8">
         <v>116</v>
       </c>
@@ -7387,7 +7603,7 @@
       <c r="G118" s="11"/>
       <c r="H118" s="11"/>
     </row>
-    <row r="119" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="119" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A119" s="8">
         <v>117</v>
       </c>
@@ -7403,7 +7619,7 @@
       <c r="G119" s="11"/>
       <c r="H119" s="11"/>
     </row>
-    <row r="120" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="120" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="8">
         <v>118</v>
       </c>
@@ -7419,7 +7635,7 @@
       <c r="G120" s="11"/>
       <c r="H120" s="11"/>
     </row>
-    <row r="121" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="121" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A121" s="8">
         <v>119</v>
       </c>
@@ -7435,7 +7651,7 @@
       <c r="G121" s="11"/>
       <c r="H121" s="11"/>
     </row>
-    <row r="122" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="122" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="8">
         <v>120</v>
       </c>
@@ -7451,7 +7667,7 @@
       <c r="G122" s="11"/>
       <c r="H122" s="11"/>
     </row>
-    <row r="123" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="123" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="8">
         <v>121</v>
       </c>
@@ -7467,7 +7683,7 @@
       <c r="G123" s="11"/>
       <c r="H123" s="11"/>
     </row>
-    <row r="124" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="124" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A124" s="8">
         <v>122</v>
       </c>
@@ -7483,7 +7699,7 @@
       <c r="G124" s="11"/>
       <c r="H124" s="11"/>
     </row>
-    <row r="125" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="125" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A125" s="8">
         <v>123</v>
       </c>
@@ -7499,7 +7715,7 @@
       <c r="G125" s="11"/>
       <c r="H125" s="11"/>
     </row>
-    <row r="126" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="126" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126" s="8">
         <v>124</v>
       </c>
@@ -7515,7 +7731,7 @@
       <c r="G126" s="11"/>
       <c r="H126" s="11"/>
     </row>
-    <row r="127" spans="1:8" ht="32.1" customHeight="1">
+    <row r="127" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A127" s="8">
         <v>125</v>
       </c>
@@ -7531,7 +7747,7 @@
       <c r="G127" s="11"/>
       <c r="H127" s="11"/>
     </row>
-    <row r="128" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="128" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A128" s="8">
         <v>126</v>
       </c>
@@ -7547,7 +7763,7 @@
       <c r="G128" s="11"/>
       <c r="H128" s="11"/>
     </row>
-    <row r="129" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="129" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="8">
         <v>127</v>
       </c>
@@ -7563,7 +7779,7 @@
       <c r="G129" s="11"/>
       <c r="H129" s="11"/>
     </row>
-    <row r="130" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="130" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="8">
         <v>128</v>
       </c>
@@ -7579,7 +7795,7 @@
       <c r="G130" s="11"/>
       <c r="H130" s="11"/>
     </row>
-    <row r="131" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="131" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="8">
         <v>129</v>
       </c>
@@ -7595,7 +7811,7 @@
       <c r="G131" s="11"/>
       <c r="H131" s="11"/>
     </row>
-    <row r="132" spans="1:8" ht="32.1" customHeight="1">
+    <row r="132" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" s="8">
         <v>130</v>
       </c>
@@ -7611,7 +7827,7 @@
       <c r="G132" s="11"/>
       <c r="H132" s="11"/>
     </row>
-    <row r="133" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="133" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" s="8">
         <v>131</v>
       </c>
@@ -7627,7 +7843,7 @@
       <c r="G133" s="11"/>
       <c r="H133" s="11"/>
     </row>
-    <row r="134" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="134" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="8">
         <v>132</v>
       </c>
@@ -7643,7 +7859,7 @@
       <c r="G134" s="11"/>
       <c r="H134" s="11"/>
     </row>
-    <row r="135" spans="1:8" ht="32.1" customHeight="1">
+    <row r="135" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A135" s="8">
         <v>133</v>
       </c>
@@ -7659,7 +7875,7 @@
       <c r="G135" s="11"/>
       <c r="H135" s="11"/>
     </row>
-    <row r="136" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="136" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="8">
         <v>134</v>
       </c>
@@ -7675,7 +7891,7 @@
       <c r="G136" s="11"/>
       <c r="H136" s="11"/>
     </row>
-    <row r="137" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="137" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A137" s="8">
         <v>135</v>
       </c>
@@ -7691,7 +7907,7 @@
       <c r="G137" s="11"/>
       <c r="H137" s="11"/>
     </row>
-    <row r="138" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="138" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A138" s="8">
         <v>136</v>
       </c>
@@ -7707,7 +7923,7 @@
       <c r="G138" s="11"/>
       <c r="H138" s="11"/>
     </row>
-    <row r="139" spans="1:8" ht="32.1" customHeight="1">
+    <row r="139" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A139" s="8">
         <v>137</v>
       </c>
@@ -7723,7 +7939,7 @@
       <c r="G139" s="11"/>
       <c r="H139" s="11"/>
     </row>
-    <row r="140" spans="1:8" ht="32.1" customHeight="1">
+    <row r="140" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="8">
         <v>138</v>
       </c>
@@ -7739,7 +7955,7 @@
       <c r="G140" s="11"/>
       <c r="H140" s="11"/>
     </row>
-    <row r="141" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="141" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A141" s="8">
         <v>139</v>
       </c>
@@ -7755,7 +7971,7 @@
       <c r="G141" s="11"/>
       <c r="H141" s="11"/>
     </row>
-    <row r="142" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="142" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="8">
         <v>140</v>
       </c>
@@ -7771,7 +7987,7 @@
       <c r="G142" s="11"/>
       <c r="H142" s="11"/>
     </row>
-    <row r="143" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="143" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A143" s="8">
         <v>141</v>
       </c>
@@ -7787,7 +8003,7 @@
       <c r="G143" s="11"/>
       <c r="H143" s="11"/>
     </row>
-    <row r="144" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="144" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" s="8">
         <v>142</v>
       </c>
@@ -7803,7 +8019,7 @@
       <c r="G144" s="11"/>
       <c r="H144" s="11"/>
     </row>
-    <row r="145" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="145" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A145" s="8">
         <v>143</v>
       </c>
@@ -7819,7 +8035,7 @@
       <c r="G145" s="11"/>
       <c r="H145" s="11"/>
     </row>
-    <row r="146" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="146" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A146" s="8">
         <v>144</v>
       </c>
@@ -7835,7 +8051,7 @@
       <c r="G146" s="11"/>
       <c r="H146" s="11"/>
     </row>
-    <row r="147" spans="1:8" ht="32.1" customHeight="1">
+    <row r="147" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A147" s="8">
         <v>145</v>
       </c>
@@ -7851,7 +8067,7 @@
       <c r="G147" s="11"/>
       <c r="H147" s="11"/>
     </row>
-    <row r="148" spans="1:8" ht="32.1" customHeight="1">
+    <row r="148" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="8">
         <v>146</v>
       </c>
@@ -7867,7 +8083,7 @@
       <c r="G148" s="11"/>
       <c r="H148" s="11"/>
     </row>
-    <row r="149" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="149" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A149" s="8">
         <v>147</v>
       </c>
@@ -7883,7 +8099,7 @@
       <c r="G149" s="11"/>
       <c r="H149" s="11"/>
     </row>
-    <row r="150" spans="1:8" ht="32.1" customHeight="1">
+    <row r="150" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A150" s="8">
         <v>148</v>
       </c>
@@ -7899,623 +8115,708 @@
       <c r="G150" s="11"/>
       <c r="H150" s="11"/>
     </row>
-    <row r="151" spans="1:8" ht="32.1" customHeight="1">
+    <row r="151" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A151" s="8">
         <v>149</v>
       </c>
       <c r="B151" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C151" s="12"/>
+      <c r="C151" s="17" t="s">
+        <v>458</v>
+      </c>
       <c r="D151" s="11"/>
       <c r="E151" s="11"/>
       <c r="F151" s="11"/>
       <c r="G151" s="11"/>
       <c r="H151" s="11"/>
     </row>
-    <row r="152" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="152" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A152" s="8">
         <v>150</v>
       </c>
       <c r="B152" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C152" s="12"/>
+      <c r="C152" s="17" t="s">
+        <v>409</v>
+      </c>
       <c r="D152" s="11"/>
       <c r="E152" s="11"/>
       <c r="F152" s="11"/>
       <c r="G152" s="11"/>
       <c r="H152" s="11"/>
     </row>
-    <row r="153" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="153" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A153" s="8">
         <v>151</v>
       </c>
       <c r="B153" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C153" s="12"/>
+      <c r="C153" s="17" t="s">
+        <v>409</v>
+      </c>
       <c r="D153" s="11"/>
       <c r="E153" s="11"/>
       <c r="F153" s="11"/>
       <c r="G153" s="11"/>
       <c r="H153" s="11"/>
     </row>
-    <row r="154" spans="1:8" ht="44.1" customHeight="1">
+    <row r="154" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A154" s="8">
         <v>152</v>
       </c>
       <c r="B154" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C154" s="12"/>
+      <c r="C154" s="17" t="s">
+        <v>459</v>
+      </c>
       <c r="D154" s="11"/>
       <c r="E154" s="11"/>
       <c r="F154" s="11"/>
       <c r="G154" s="11"/>
       <c r="H154" s="11"/>
     </row>
-    <row r="155" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="155" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A155" s="8">
         <v>153</v>
       </c>
       <c r="B155" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C155" s="12"/>
+      <c r="C155" s="17" t="s">
+        <v>459</v>
+      </c>
       <c r="D155" s="11"/>
       <c r="E155" s="11"/>
       <c r="F155" s="11"/>
       <c r="G155" s="11"/>
       <c r="H155" s="11"/>
     </row>
-    <row r="156" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="156" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A156" s="8">
         <v>154</v>
       </c>
       <c r="B156" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C156" s="12"/>
+      <c r="C156" s="17" t="s">
+        <v>460</v>
+      </c>
       <c r="D156" s="11"/>
       <c r="E156" s="11"/>
       <c r="F156" s="11"/>
       <c r="G156" s="11"/>
       <c r="H156" s="11"/>
     </row>
-    <row r="157" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="157" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A157" s="8">
         <v>155</v>
       </c>
       <c r="B157" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C157" s="12"/>
+      <c r="C157" s="17" t="s">
+        <v>459</v>
+      </c>
       <c r="D157" s="11"/>
       <c r="E157" s="11"/>
       <c r="F157" s="11"/>
       <c r="G157" s="11"/>
       <c r="H157" s="11"/>
     </row>
-    <row r="158" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="158" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A158" s="8">
         <v>156</v>
       </c>
       <c r="B158" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C158" s="12"/>
+      <c r="C158" s="17" t="s">
+        <v>461</v>
+      </c>
       <c r="D158" s="11"/>
       <c r="E158" s="11"/>
       <c r="F158" s="11"/>
       <c r="G158" s="11"/>
       <c r="H158" s="11"/>
     </row>
-    <row r="159" spans="1:8" ht="32.1" customHeight="1">
+    <row r="159" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A159" s="8">
         <v>157</v>
       </c>
       <c r="B159" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C159" s="12"/>
+      <c r="C159" s="17" t="s">
+        <v>462</v>
+      </c>
       <c r="D159" s="11"/>
       <c r="E159" s="11"/>
       <c r="F159" s="11"/>
       <c r="G159" s="11"/>
       <c r="H159" s="11"/>
     </row>
-    <row r="160" spans="1:8" ht="44.1" customHeight="1">
+    <row r="160" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A160" s="8">
         <v>158</v>
       </c>
       <c r="B160" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C160" s="12"/>
+      <c r="C160" s="17" t="s">
+        <v>459</v>
+      </c>
       <c r="D160" s="11"/>
       <c r="E160" s="11"/>
       <c r="F160" s="11"/>
       <c r="G160" s="11"/>
       <c r="H160" s="11"/>
     </row>
-    <row r="161" spans="1:8" ht="44.1" customHeight="1">
+    <row r="161" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A161" s="8">
         <v>159</v>
       </c>
       <c r="B161" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C161" s="12"/>
+      <c r="C161" s="17" t="s">
+        <v>459</v>
+      </c>
       <c r="D161" s="11"/>
       <c r="E161" s="11"/>
       <c r="F161" s="11"/>
       <c r="G161" s="11"/>
       <c r="H161" s="11"/>
     </row>
-    <row r="162" spans="1:8" ht="32.1" customHeight="1">
+    <row r="162" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A162" s="8">
         <v>160</v>
       </c>
       <c r="B162" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C162" s="12"/>
+      <c r="C162" s="17" t="s">
+        <v>459</v>
+      </c>
       <c r="D162" s="11"/>
       <c r="E162" s="11"/>
       <c r="F162" s="11"/>
       <c r="G162" s="11"/>
       <c r="H162" s="11"/>
     </row>
-    <row r="163" spans="1:8" ht="32.1" customHeight="1">
+    <row r="163" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A163" s="8">
         <v>161</v>
       </c>
       <c r="B163" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C163" s="12"/>
+      <c r="C163" s="17" t="s">
+        <v>463</v>
+      </c>
       <c r="D163" s="11"/>
       <c r="E163" s="11"/>
       <c r="F163" s="11"/>
       <c r="G163" s="11"/>
       <c r="H163" s="11"/>
     </row>
-    <row r="164" spans="1:8" ht="32.1" customHeight="1">
+    <row r="164" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A164" s="8">
         <v>162</v>
       </c>
       <c r="B164" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C164" s="12"/>
+      <c r="C164" s="17" t="s">
+        <v>464</v>
+      </c>
       <c r="D164" s="11"/>
       <c r="E164" s="11"/>
       <c r="F164" s="11"/>
       <c r="G164" s="11"/>
       <c r="H164" s="11"/>
     </row>
-    <row r="165" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="165" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A165" s="8">
         <v>163</v>
       </c>
       <c r="B165" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C165" s="12"/>
+      <c r="C165" s="17" t="s">
+        <v>465</v>
+      </c>
       <c r="D165" s="11"/>
       <c r="E165" s="11"/>
       <c r="F165" s="11"/>
       <c r="G165" s="11"/>
       <c r="H165" s="11"/>
     </row>
-    <row r="166" spans="1:8" ht="32.1" customHeight="1">
+    <row r="166" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A166" s="8">
         <v>164</v>
       </c>
       <c r="B166" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C166" s="12"/>
+      <c r="C166" s="17" t="s">
+        <v>466</v>
+      </c>
       <c r="D166" s="11"/>
       <c r="E166" s="11"/>
       <c r="F166" s="11"/>
       <c r="G166" s="11"/>
       <c r="H166" s="11"/>
     </row>
-    <row r="167" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="167" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A167" s="8">
         <v>165</v>
       </c>
       <c r="B167" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C167" s="12"/>
+      <c r="C167" s="17" t="s">
+        <v>318</v>
+      </c>
       <c r="D167" s="11"/>
       <c r="E167" s="11"/>
       <c r="F167" s="11"/>
       <c r="G167" s="11"/>
       <c r="H167" s="11"/>
     </row>
-    <row r="168" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="168" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A168" s="8">
         <v>166</v>
       </c>
       <c r="B168" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="C168" s="10"/>
+      <c r="C168" s="18" t="s">
+        <v>467</v>
+      </c>
       <c r="D168" s="11"/>
       <c r="E168" s="11"/>
       <c r="F168" s="11"/>
       <c r="G168" s="11"/>
       <c r="H168" s="11"/>
     </row>
-    <row r="169" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="169" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A169" s="8">
         <v>167</v>
       </c>
       <c r="B169" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="C169" s="12"/>
+      <c r="C169" s="17" t="s">
+        <v>468</v>
+      </c>
       <c r="D169" s="11"/>
       <c r="E169" s="11"/>
       <c r="F169" s="11"/>
       <c r="G169" s="11"/>
       <c r="H169" s="11"/>
     </row>
-    <row r="170" spans="1:8" ht="32.1" customHeight="1">
+    <row r="170" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A170" s="8">
         <v>168</v>
       </c>
       <c r="B170" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C170" s="12"/>
+      <c r="C170" s="17" t="s">
+        <v>469</v>
+      </c>
       <c r="D170" s="11"/>
       <c r="E170" s="11"/>
       <c r="F170" s="11"/>
       <c r="G170" s="11"/>
       <c r="H170" s="11"/>
     </row>
-    <row r="171" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="171" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A171" s="8">
         <v>169</v>
       </c>
       <c r="B171" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C171" s="12"/>
+      <c r="C171" s="17" t="s">
+        <v>470</v>
+      </c>
       <c r="D171" s="11"/>
       <c r="E171" s="11"/>
       <c r="F171" s="11"/>
       <c r="G171" s="11"/>
       <c r="H171" s="11"/>
     </row>
-    <row r="172" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="172" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A172" s="8">
         <v>170</v>
       </c>
       <c r="B172" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="C172" s="12"/>
+      <c r="C172" s="17" t="s">
+        <v>471</v>
+      </c>
       <c r="D172" s="11"/>
       <c r="E172" s="11"/>
       <c r="F172" s="11"/>
       <c r="G172" s="11"/>
       <c r="H172" s="11"/>
     </row>
-    <row r="173" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="173" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A173" s="8">
         <v>171</v>
       </c>
       <c r="B173" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C173" s="12"/>
+      <c r="C173" s="17" t="s">
+        <v>472</v>
+      </c>
       <c r="D173" s="11"/>
       <c r="E173" s="11"/>
       <c r="F173" s="11"/>
       <c r="G173" s="11"/>
       <c r="H173" s="11"/>
     </row>
-    <row r="174" spans="1:8" ht="32.1" customHeight="1">
+    <row r="174" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A174" s="8">
         <v>172</v>
       </c>
       <c r="B174" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C174" s="12"/>
+      <c r="C174" s="17" t="s">
+        <v>473</v>
+      </c>
       <c r="D174" s="11"/>
       <c r="E174" s="11"/>
       <c r="F174" s="11"/>
       <c r="G174" s="11"/>
       <c r="H174" s="11"/>
     </row>
-    <row r="175" spans="1:8" ht="32.1" customHeight="1">
+    <row r="175" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A175" s="8">
         <v>173</v>
       </c>
       <c r="B175" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C175" s="12"/>
+      <c r="C175" s="17" t="s">
+        <v>474</v>
+      </c>
       <c r="D175" s="11"/>
       <c r="E175" s="11"/>
       <c r="F175" s="11"/>
       <c r="G175" s="11"/>
       <c r="H175" s="11"/>
     </row>
-    <row r="176" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="176" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A176" s="8">
         <v>174</v>
       </c>
       <c r="B176" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="C176" s="12"/>
+      <c r="C176" s="17" t="s">
+        <v>475</v>
+      </c>
       <c r="D176" s="11"/>
       <c r="E176" s="11"/>
       <c r="F176" s="11"/>
       <c r="G176" s="11"/>
       <c r="H176" s="11"/>
     </row>
-    <row r="177" spans="1:8" ht="44.1" customHeight="1">
+    <row r="177" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A177" s="8">
         <v>175</v>
       </c>
       <c r="B177" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C177" s="12"/>
+      <c r="C177" s="17" t="s">
+        <v>476</v>
+      </c>
       <c r="D177" s="11"/>
       <c r="E177" s="11"/>
       <c r="F177" s="11"/>
       <c r="G177" s="11"/>
       <c r="H177" s="11"/>
     </row>
-    <row r="178" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="178" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A178" s="8">
         <v>176</v>
       </c>
       <c r="B178" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="C178" s="12"/>
+      <c r="C178" s="17" t="s">
+        <v>455</v>
+      </c>
       <c r="D178" s="11"/>
       <c r="E178" s="11"/>
       <c r="F178" s="11"/>
       <c r="G178" s="11"/>
       <c r="H178" s="11"/>
     </row>
-    <row r="179" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="179" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A179" s="8">
         <v>177</v>
       </c>
       <c r="B179" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C179" s="10"/>
+      <c r="C179" s="18" t="s">
+        <v>477</v>
+      </c>
       <c r="D179" s="11"/>
       <c r="E179" s="11"/>
       <c r="F179" s="11"/>
       <c r="G179" s="11"/>
       <c r="H179" s="11"/>
     </row>
-    <row r="180" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="180" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A180" s="8">
         <v>178</v>
       </c>
       <c r="B180" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C180" s="12"/>
+      <c r="C180" s="17" t="s">
+        <v>478</v>
+      </c>
       <c r="D180" s="11"/>
       <c r="E180" s="11"/>
       <c r="F180" s="11"/>
       <c r="G180" s="11"/>
       <c r="H180" s="11"/>
     </row>
-    <row r="181" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="181" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A181" s="8">
         <v>179</v>
       </c>
       <c r="B181" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C181" s="12"/>
+      <c r="C181" s="17" t="s">
+        <v>479</v>
+      </c>
       <c r="D181" s="11"/>
       <c r="E181" s="11"/>
       <c r="F181" s="11"/>
       <c r="G181" s="11"/>
       <c r="H181" s="11"/>
     </row>
-    <row r="182" spans="1:8" ht="56.1" customHeight="1">
+    <row r="182" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A182" s="8">
         <v>180</v>
       </c>
       <c r="B182" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C182" s="12"/>
+      <c r="C182" s="17" t="s">
+        <v>480</v>
+      </c>
       <c r="D182" s="11"/>
       <c r="E182" s="11"/>
       <c r="F182" s="11"/>
       <c r="G182" s="11"/>
       <c r="H182" s="11"/>
     </row>
-    <row r="183" spans="1:8" ht="32.1" customHeight="1">
+    <row r="183" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A183" s="8">
         <v>181</v>
       </c>
       <c r="B183" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C183" s="12"/>
+      <c r="C183" s="17" t="s">
+        <v>318</v>
+      </c>
       <c r="D183" s="11"/>
       <c r="E183" s="11"/>
       <c r="F183" s="11"/>
       <c r="G183" s="11"/>
       <c r="H183" s="11"/>
     </row>
-    <row r="184" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="184" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A184" s="8">
         <v>182</v>
       </c>
       <c r="B184" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C184" s="12"/>
+      <c r="C184" s="17" t="s">
+        <v>318</v>
+      </c>
       <c r="D184" s="11"/>
       <c r="E184" s="11"/>
       <c r="F184" s="11"/>
       <c r="G184" s="11"/>
       <c r="H184" s="11"/>
     </row>
-    <row r="185" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="185" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A185" s="8">
         <v>183</v>
       </c>
       <c r="B185" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C185" s="10"/>
+      <c r="C185" s="18" t="s">
+        <v>398</v>
+      </c>
       <c r="D185" s="11"/>
       <c r="E185" s="11"/>
       <c r="F185" s="11"/>
       <c r="G185" s="11"/>
       <c r="H185" s="11"/>
     </row>
-    <row r="186" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="186" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A186" s="8">
         <v>184</v>
       </c>
       <c r="B186" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C186" s="12"/>
+      <c r="C186" s="17" t="s">
+        <v>318</v>
+      </c>
       <c r="D186" s="11"/>
       <c r="E186" s="11"/>
       <c r="F186" s="11"/>
       <c r="G186" s="11"/>
       <c r="H186" s="11"/>
     </row>
-    <row r="187" spans="1:8" ht="56.1" customHeight="1">
+    <row r="187" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A187" s="8">
         <v>185</v>
       </c>
       <c r="B187" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="C187" s="12"/>
+      <c r="C187" s="17" t="s">
+        <v>481</v>
+      </c>
       <c r="D187" s="11"/>
       <c r="E187" s="11"/>
       <c r="F187" s="11"/>
       <c r="G187" s="11"/>
       <c r="H187" s="11"/>
     </row>
-    <row r="188" spans="1:8" ht="32.1" customHeight="1">
+    <row r="188" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A188" s="8">
         <v>186</v>
       </c>
       <c r="B188" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C188" s="12"/>
+      <c r="C188" s="17" t="s">
+        <v>455</v>
+      </c>
       <c r="D188" s="11"/>
       <c r="E188" s="11"/>
       <c r="F188" s="11"/>
       <c r="G188" s="11"/>
       <c r="H188" s="11"/>
     </row>
-    <row r="189" spans="1:8" ht="32.1" customHeight="1">
+    <row r="189" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A189" s="8">
         <v>187</v>
       </c>
       <c r="B189" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="C189" s="12"/>
+      <c r="C189" s="17" t="s">
+        <v>455</v>
+      </c>
       <c r="D189" s="11"/>
       <c r="E189" s="11"/>
       <c r="F189" s="11"/>
       <c r="G189" s="11"/>
       <c r="H189" s="11"/>
     </row>
-    <row r="190" spans="1:8" ht="32.1" customHeight="1">
+    <row r="190" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A190" s="8">
         <v>188</v>
       </c>
       <c r="B190" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C190" s="12"/>
+      <c r="C190" s="17" t="s">
+        <v>455</v>
+      </c>
       <c r="D190" s="11"/>
       <c r="E190" s="11"/>
       <c r="F190" s="11"/>
       <c r="G190" s="11"/>
       <c r="H190" s="11"/>
     </row>
-    <row r="191" spans="1:8" ht="56.1" customHeight="1">
+    <row r="191" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A191" s="8">
         <v>189</v>
       </c>
       <c r="B191" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C191" s="12"/>
+      <c r="C191" s="17" t="s">
+        <v>482</v>
+      </c>
       <c r="D191" s="11"/>
       <c r="E191" s="11"/>
       <c r="F191" s="11"/>
       <c r="G191" s="11"/>
       <c r="H191" s="11"/>
     </row>
-    <row r="192" spans="1:8" ht="32.1" customHeight="1">
+    <row r="192" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A192" s="8">
         <v>190</v>
       </c>
       <c r="B192" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="C192" s="12"/>
+      <c r="C192" s="17" t="s">
+        <v>483</v>
+      </c>
       <c r="D192" s="11"/>
       <c r="E192" s="11"/>
       <c r="F192" s="11"/>
       <c r="G192" s="11"/>
       <c r="H192" s="11"/>
     </row>
-    <row r="193" spans="1:8" ht="32.1" customHeight="1">
+    <row r="193" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A193" s="8">
         <v>191</v>
       </c>
       <c r="B193" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="C193" s="12"/>
+      <c r="C193" s="17" t="s">
+        <v>475</v>
+      </c>
       <c r="D193" s="11"/>
       <c r="E193" s="11"/>
       <c r="F193" s="11"/>
       <c r="G193" s="11"/>
       <c r="H193" s="11"/>
     </row>
-    <row r="194" spans="1:8" ht="32.1" customHeight="1">
+    <row r="194" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A194" s="8">
         <v>192</v>
       </c>
       <c r="B194" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C194" s="12"/>
       <c r="D194" s="11"/>
       <c r="E194" s="11"/>
       <c r="F194" s="11"/>
       <c r="G194" s="11"/>
       <c r="H194" s="11"/>
     </row>
-    <row r="195" spans="1:8" ht="32.1" customHeight="1">
+    <row r="195" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A195" s="8">
         <v>193</v>
       </c>
@@ -8529,637 +8830,724 @@
       <c r="G195" s="11"/>
       <c r="H195" s="11"/>
     </row>
-    <row r="196" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="196" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A196" s="8">
         <v>194</v>
       </c>
       <c r="B196" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C196" s="12"/>
+      <c r="C196" s="17" t="s">
+        <v>484</v>
+      </c>
       <c r="D196" s="11"/>
       <c r="E196" s="11"/>
       <c r="F196" s="11"/>
       <c r="G196" s="11"/>
       <c r="H196" s="11"/>
     </row>
-    <row r="197" spans="1:8" ht="56.1" customHeight="1">
+    <row r="197" spans="1:8" ht="56" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A197" s="8">
         <v>195</v>
       </c>
       <c r="B197" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C197" s="12"/>
+      <c r="C197" s="17" t="s">
+        <v>485</v>
+      </c>
       <c r="D197" s="11"/>
       <c r="E197" s="11"/>
       <c r="F197" s="11"/>
       <c r="G197" s="11"/>
       <c r="H197" s="11"/>
     </row>
-    <row r="198" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="198" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A198" s="8">
         <v>196</v>
       </c>
       <c r="B198" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C198" s="12"/>
+      <c r="C198" s="17" t="s">
+        <v>486</v>
+      </c>
       <c r="D198" s="11"/>
       <c r="E198" s="11"/>
       <c r="F198" s="11"/>
       <c r="G198" s="11"/>
       <c r="H198" s="11"/>
     </row>
-    <row r="199" spans="1:8" ht="32.1" customHeight="1">
+    <row r="199" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A199" s="8">
         <v>197</v>
       </c>
       <c r="B199" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C199" s="12"/>
+      <c r="C199" s="17" t="s">
+        <v>487</v>
+      </c>
       <c r="D199" s="11"/>
       <c r="E199" s="11"/>
       <c r="F199" s="11"/>
       <c r="G199" s="11"/>
       <c r="H199" s="11"/>
     </row>
-    <row r="200" spans="1:8" ht="32.1" customHeight="1">
+    <row r="200" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A200" s="8">
         <v>198</v>
       </c>
       <c r="B200" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C200" s="12"/>
+      <c r="C200" s="17" t="s">
+        <v>488</v>
+      </c>
       <c r="D200" s="11"/>
       <c r="E200" s="11"/>
       <c r="F200" s="11"/>
       <c r="G200" s="11"/>
       <c r="H200" s="11"/>
     </row>
-    <row r="201" spans="1:8" ht="32.1" customHeight="1">
+    <row r="201" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A201" s="8">
         <v>199</v>
       </c>
       <c r="B201" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C201" s="12"/>
+      <c r="C201" s="17" t="s">
+        <v>489</v>
+      </c>
       <c r="D201" s="11"/>
       <c r="E201" s="11"/>
       <c r="F201" s="11"/>
       <c r="G201" s="11"/>
       <c r="H201" s="11"/>
     </row>
-    <row r="202" spans="1:8" ht="32.1" customHeight="1">
+    <row r="202" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A202" s="8">
         <v>200</v>
       </c>
       <c r="B202" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C202" s="12"/>
+      <c r="C202" s="17" t="s">
+        <v>491</v>
+      </c>
       <c r="D202" s="11"/>
       <c r="E202" s="11"/>
       <c r="F202" s="11"/>
       <c r="G202" s="11"/>
       <c r="H202" s="11"/>
     </row>
-    <row r="203" spans="1:8" ht="32.1" customHeight="1">
+    <row r="203" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A203" s="8">
         <v>201</v>
       </c>
       <c r="B203" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C203" s="12"/>
+      <c r="C203" s="17" t="s">
+        <v>490</v>
+      </c>
       <c r="D203" s="11"/>
       <c r="E203" s="11"/>
       <c r="F203" s="11"/>
       <c r="G203" s="11"/>
       <c r="H203" s="11"/>
     </row>
-    <row r="204" spans="1:8" ht="32.1" customHeight="1">
+    <row r="204" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A204" s="8">
         <v>202</v>
       </c>
       <c r="B204" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C204" s="12"/>
+      <c r="C204" s="17" t="s">
+        <v>492</v>
+      </c>
       <c r="D204" s="11"/>
       <c r="E204" s="11"/>
       <c r="F204" s="11"/>
       <c r="G204" s="11"/>
       <c r="H204" s="11"/>
     </row>
-    <row r="205" spans="1:8" ht="32.1" customHeight="1">
+    <row r="205" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A205" s="8">
         <v>203</v>
       </c>
       <c r="B205" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C205" s="12"/>
+      <c r="C205" s="17" t="s">
+        <v>398</v>
+      </c>
       <c r="D205" s="11"/>
       <c r="E205" s="11"/>
       <c r="F205" s="11"/>
       <c r="G205" s="11"/>
       <c r="H205" s="11"/>
     </row>
-    <row r="206" spans="1:8" ht="32.1" customHeight="1">
+    <row r="206" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A206" s="8">
         <v>204</v>
       </c>
       <c r="B206" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C206" s="12"/>
+      <c r="C206" s="17" t="s">
+        <v>318</v>
+      </c>
       <c r="D206" s="11"/>
       <c r="E206" s="11"/>
       <c r="F206" s="11"/>
       <c r="G206" s="11"/>
       <c r="H206" s="11"/>
     </row>
-    <row r="207" spans="1:8" ht="32.1" customHeight="1">
+    <row r="207" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A207" s="8">
         <v>205</v>
       </c>
       <c r="B207" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C207" s="12"/>
+      <c r="C207" s="17" t="s">
+        <v>493</v>
+      </c>
       <c r="D207" s="11"/>
       <c r="E207" s="11"/>
       <c r="F207" s="11"/>
       <c r="G207" s="11"/>
       <c r="H207" s="11"/>
     </row>
-    <row r="208" spans="1:8" ht="32.1" customHeight="1">
+    <row r="208" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A208" s="8">
         <v>206</v>
       </c>
       <c r="B208" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C208" s="12"/>
+      <c r="C208" s="17" t="s">
+        <v>494</v>
+      </c>
       <c r="D208" s="11"/>
       <c r="E208" s="11"/>
       <c r="F208" s="11"/>
       <c r="G208" s="11"/>
       <c r="H208" s="11"/>
     </row>
-    <row r="209" spans="1:8" ht="32.1" customHeight="1">
+    <row r="209" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A209" s="8">
         <v>207</v>
       </c>
       <c r="B209" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="C209" s="12"/>
+      <c r="C209" s="17" t="s">
+        <v>495</v>
+      </c>
       <c r="D209" s="11"/>
       <c r="E209" s="11"/>
       <c r="F209" s="11"/>
       <c r="G209" s="11"/>
       <c r="H209" s="11"/>
     </row>
-    <row r="210" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="210" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A210" s="8">
         <v>208</v>
       </c>
       <c r="B210" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C210" s="12"/>
+      <c r="C210" s="17" t="s">
+        <v>496</v>
+      </c>
       <c r="D210" s="11"/>
       <c r="E210" s="11"/>
       <c r="F210" s="11"/>
       <c r="G210" s="11"/>
       <c r="H210" s="11"/>
     </row>
-    <row r="211" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="211" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A211" s="8">
         <v>209</v>
       </c>
       <c r="B211" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C211" s="10"/>
+      <c r="C211" s="18" t="s">
+        <v>497</v>
+      </c>
       <c r="D211" s="11"/>
       <c r="E211" s="11"/>
       <c r="F211" s="11"/>
       <c r="G211" s="11"/>
       <c r="H211" s="11"/>
     </row>
-    <row r="212" spans="1:8" ht="32.1" customHeight="1">
+    <row r="212" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A212" s="8">
         <v>210</v>
       </c>
       <c r="B212" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C212" s="12"/>
+      <c r="C212" s="17" t="s">
+        <v>496</v>
+      </c>
       <c r="D212" s="11"/>
       <c r="E212" s="11"/>
       <c r="F212" s="11"/>
       <c r="G212" s="11"/>
       <c r="H212" s="11"/>
     </row>
-    <row r="213" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="213" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A213" s="8">
         <v>211</v>
       </c>
       <c r="B213" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C213" s="10"/>
       <c r="D213" s="11"/>
       <c r="E213" s="11"/>
       <c r="F213" s="11"/>
       <c r="G213" s="11"/>
       <c r="H213" s="11"/>
     </row>
-    <row r="214" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="214" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A214" s="8">
         <v>212</v>
       </c>
       <c r="B214" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="C214" s="10"/>
+      <c r="C214" s="18" t="s">
+        <v>398</v>
+      </c>
       <c r="D214" s="11"/>
       <c r="E214" s="11"/>
       <c r="F214" s="11"/>
       <c r="G214" s="11"/>
       <c r="H214" s="11"/>
     </row>
-    <row r="215" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="215" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A215" s="8">
         <v>213</v>
       </c>
       <c r="B215" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C215" s="12"/>
+      <c r="C215" s="17" t="s">
+        <v>498</v>
+      </c>
       <c r="D215" s="11"/>
       <c r="E215" s="11"/>
       <c r="F215" s="11"/>
       <c r="G215" s="11"/>
       <c r="H215" s="11"/>
     </row>
-    <row r="216" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="216" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A216" s="8">
         <v>214</v>
       </c>
       <c r="B216" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="C216" s="12"/>
+      <c r="C216" s="17" t="s">
+        <v>499</v>
+      </c>
       <c r="D216" s="11"/>
       <c r="E216" s="11"/>
       <c r="F216" s="11"/>
       <c r="G216" s="11"/>
       <c r="H216" s="11"/>
     </row>
-    <row r="217" spans="1:8" ht="32.1" customHeight="1">
+    <row r="217" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A217" s="8">
         <v>215</v>
       </c>
       <c r="B217" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="C217" s="12"/>
+      <c r="C217" s="17" t="s">
+        <v>500</v>
+      </c>
       <c r="D217" s="11"/>
       <c r="E217" s="11"/>
       <c r="F217" s="11"/>
       <c r="G217" s="11"/>
       <c r="H217" s="11"/>
     </row>
-    <row r="218" spans="1:8" ht="32.1" customHeight="1">
+    <row r="218" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A218" s="8">
         <v>216</v>
       </c>
       <c r="B218" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="C218" s="12"/>
+      <c r="C218" s="17" t="s">
+        <v>501</v>
+      </c>
       <c r="D218" s="11"/>
       <c r="E218" s="11"/>
       <c r="F218" s="11"/>
       <c r="G218" s="11"/>
       <c r="H218" s="11"/>
     </row>
-    <row r="219" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="219" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A219" s="8">
         <v>217</v>
       </c>
       <c r="B219" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C219" s="12"/>
+      <c r="C219" s="17" t="s">
+        <v>502</v>
+      </c>
       <c r="D219" s="11"/>
       <c r="E219" s="11"/>
       <c r="F219" s="11"/>
       <c r="G219" s="11"/>
       <c r="H219" s="11"/>
     </row>
-    <row r="220" spans="1:8" ht="32.1" customHeight="1">
+    <row r="220" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A220" s="8">
         <v>218</v>
       </c>
       <c r="B220" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C220" s="12"/>
+      <c r="C220" s="17" t="s">
+        <v>503</v>
+      </c>
       <c r="D220" s="11"/>
       <c r="E220" s="11"/>
       <c r="F220" s="11"/>
       <c r="G220" s="11"/>
       <c r="H220" s="11"/>
     </row>
-    <row r="221" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="221" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A221" s="8">
         <v>219</v>
       </c>
       <c r="B221" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C221" s="10"/>
+      <c r="C221" s="18" t="s">
+        <v>504</v>
+      </c>
       <c r="D221" s="11"/>
       <c r="E221" s="11"/>
       <c r="F221" s="11"/>
       <c r="G221" s="11"/>
       <c r="H221" s="11"/>
     </row>
-    <row r="222" spans="1:8" ht="32.1" customHeight="1">
+    <row r="222" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A222" s="8">
         <v>220</v>
       </c>
       <c r="B222" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="C222" s="12"/>
+      <c r="C222" s="17" t="s">
+        <v>505</v>
+      </c>
       <c r="D222" s="11"/>
       <c r="E222" s="11"/>
       <c r="F222" s="11"/>
       <c r="G222" s="11"/>
       <c r="H222" s="11"/>
     </row>
-    <row r="223" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="223" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A223" s="8">
         <v>221</v>
       </c>
       <c r="B223" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="C223" s="12"/>
+      <c r="C223" s="17" t="s">
+        <v>318</v>
+      </c>
       <c r="D223" s="11"/>
       <c r="E223" s="11"/>
       <c r="F223" s="11"/>
       <c r="G223" s="11"/>
       <c r="H223" s="11"/>
     </row>
-    <row r="224" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="224" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A224" s="8">
         <v>222</v>
       </c>
       <c r="B224" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="C224" s="12"/>
+      <c r="C224" s="17" t="s">
+        <v>318</v>
+      </c>
       <c r="D224" s="11"/>
       <c r="E224" s="11"/>
       <c r="F224" s="11"/>
       <c r="G224" s="11"/>
       <c r="H224" s="11"/>
     </row>
-    <row r="225" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="225" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A225" s="8">
         <v>223</v>
       </c>
       <c r="B225" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C225" s="12"/>
+      <c r="C225" s="17" t="s">
+        <v>506</v>
+      </c>
       <c r="D225" s="11"/>
       <c r="E225" s="11"/>
       <c r="F225" s="11"/>
       <c r="G225" s="11"/>
       <c r="H225" s="11"/>
     </row>
-    <row r="226" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="226" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A226" s="8">
         <v>224</v>
       </c>
       <c r="B226" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="C226" s="12"/>
+      <c r="C226" s="17" t="s">
+        <v>318</v>
+      </c>
       <c r="D226" s="11"/>
       <c r="E226" s="11"/>
       <c r="F226" s="11"/>
       <c r="G226" s="11"/>
       <c r="H226" s="11"/>
     </row>
-    <row r="227" spans="1:8" ht="32.1" customHeight="1">
+    <row r="227" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A227" s="8">
         <v>225</v>
       </c>
       <c r="B227" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="C227" s="12"/>
+      <c r="C227" s="17" t="s">
+        <v>507</v>
+      </c>
       <c r="D227" s="11"/>
       <c r="E227" s="11"/>
       <c r="F227" s="11"/>
       <c r="G227" s="11"/>
       <c r="H227" s="11"/>
     </row>
-    <row r="228" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="228" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A228" s="8">
         <v>226</v>
       </c>
       <c r="B228" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C228" s="12"/>
+      <c r="C228" s="17" t="s">
+        <v>508</v>
+      </c>
       <c r="D228" s="11"/>
       <c r="E228" s="11"/>
       <c r="F228" s="11"/>
       <c r="G228" s="11"/>
       <c r="H228" s="11"/>
     </row>
-    <row r="229" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="229" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A229" s="8">
         <v>227</v>
       </c>
       <c r="B229" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="C229" s="12"/>
+      <c r="C229" s="17" t="s">
+        <v>509</v>
+      </c>
       <c r="D229" s="11"/>
       <c r="E229" s="11"/>
       <c r="F229" s="11"/>
       <c r="G229" s="11"/>
       <c r="H229" s="11"/>
     </row>
-    <row r="230" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="230" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A230" s="8">
         <v>228</v>
       </c>
       <c r="B230" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="C230" s="12"/>
+      <c r="C230" s="17" t="s">
+        <v>318</v>
+      </c>
       <c r="D230" s="11"/>
       <c r="E230" s="11"/>
       <c r="F230" s="11"/>
       <c r="G230" s="11"/>
       <c r="H230" s="11"/>
     </row>
-    <row r="231" spans="1:8" ht="32.1" customHeight="1">
+    <row r="231" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A231" s="8">
         <v>229</v>
       </c>
       <c r="B231" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="C231" s="12"/>
+      <c r="C231" s="17" t="s">
+        <v>510</v>
+      </c>
       <c r="D231" s="11"/>
       <c r="E231" s="11"/>
       <c r="F231" s="11"/>
       <c r="G231" s="11"/>
       <c r="H231" s="11"/>
     </row>
-    <row r="232" spans="1:8" ht="44.1" customHeight="1">
+    <row r="232" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A232" s="8">
         <v>230</v>
       </c>
       <c r="B232" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="C232" s="12"/>
+      <c r="C232" s="17" t="s">
+        <v>511</v>
+      </c>
       <c r="D232" s="11"/>
       <c r="E232" s="11"/>
       <c r="F232" s="11"/>
       <c r="G232" s="11"/>
       <c r="H232" s="11"/>
     </row>
-    <row r="233" spans="1:8" ht="32.1" customHeight="1">
+    <row r="233" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A233" s="8">
         <v>231</v>
       </c>
       <c r="B233" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C233" s="12"/>
+      <c r="C233" s="17" t="s">
+        <v>512</v>
+      </c>
       <c r="D233" s="11"/>
       <c r="E233" s="11"/>
       <c r="F233" s="11"/>
       <c r="G233" s="11"/>
       <c r="H233" s="11"/>
     </row>
-    <row r="234" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="234" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A234" s="8">
         <v>232</v>
       </c>
       <c r="B234" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="C234" s="12"/>
+      <c r="C234" s="17" t="s">
+        <v>513</v>
+      </c>
       <c r="D234" s="11"/>
       <c r="E234" s="11"/>
       <c r="F234" s="11"/>
       <c r="G234" s="11"/>
       <c r="H234" s="11"/>
     </row>
-    <row r="235" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="235" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A235" s="8">
         <v>233</v>
       </c>
       <c r="B235" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="C235" s="12"/>
+      <c r="C235" s="17" t="s">
+        <v>514</v>
+      </c>
       <c r="D235" s="11"/>
       <c r="E235" s="11"/>
       <c r="F235" s="11"/>
       <c r="G235" s="11"/>
       <c r="H235" s="11"/>
     </row>
-    <row r="236" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="236" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A236" s="8">
         <v>234</v>
       </c>
       <c r="B236" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="C236" s="12"/>
+      <c r="C236" s="12" t="s">
+        <v>514</v>
+      </c>
       <c r="D236" s="11"/>
       <c r="E236" s="11"/>
       <c r="F236" s="11"/>
       <c r="G236" s="11"/>
       <c r="H236" s="11"/>
     </row>
-    <row r="237" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="237" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A237" s="8">
         <v>235</v>
       </c>
       <c r="B237" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C237" s="12"/>
+      <c r="C237" s="17" t="s">
+        <v>366</v>
+      </c>
       <c r="D237" s="11"/>
       <c r="E237" s="11"/>
       <c r="F237" s="11"/>
       <c r="G237" s="11"/>
       <c r="H237" s="11"/>
     </row>
-    <row r="238" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="238" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A238" s="8">
         <v>236</v>
       </c>
       <c r="B238" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="C238" s="12"/>
+      <c r="C238" s="17" t="s">
+        <v>366</v>
+      </c>
       <c r="D238" s="11"/>
       <c r="E238" s="11"/>
       <c r="F238" s="11"/>
       <c r="G238" s="11"/>
       <c r="H238" s="11"/>
     </row>
-    <row r="239" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="239" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A239" s="8">
         <v>237</v>
       </c>
       <c r="B239" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="C239" s="12"/>
+      <c r="C239" s="17" t="s">
+        <v>366</v>
+      </c>
       <c r="D239" s="11"/>
       <c r="E239" s="11"/>
       <c r="F239" s="11"/>
       <c r="G239" s="11"/>
       <c r="H239" s="11"/>
     </row>
-    <row r="240" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="240" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A240" s="8">
         <v>238</v>
       </c>
       <c r="B240" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="C240" s="12"/>
+      <c r="C240" s="17" t="s">
+        <v>366</v>
+      </c>
       <c r="D240" s="11"/>
       <c r="E240" s="11"/>
       <c r="F240" s="11"/>
       <c r="G240" s="11"/>
       <c r="H240" s="11"/>
     </row>
-    <row r="241" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="241" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A241" s="8">
         <v>239</v>
       </c>
@@ -9173,35 +9561,39 @@
       <c r="G241" s="11"/>
       <c r="H241" s="11"/>
     </row>
-    <row r="242" spans="1:8" ht="32.1" customHeight="1">
+    <row r="242" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A242" s="8">
         <v>240</v>
       </c>
       <c r="B242" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C242" s="12"/>
+      <c r="C242" s="17" t="s">
+        <v>515</v>
+      </c>
       <c r="D242" s="11"/>
       <c r="E242" s="11"/>
       <c r="F242" s="11"/>
       <c r="G242" s="11"/>
       <c r="H242" s="11"/>
     </row>
-    <row r="243" spans="1:8" ht="32.1" customHeight="1">
+    <row r="243" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A243" s="8">
         <v>241</v>
       </c>
       <c r="B243" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C243" s="12"/>
+      <c r="C243" s="17" t="s">
+        <v>516</v>
+      </c>
       <c r="D243" s="11"/>
       <c r="E243" s="11"/>
       <c r="F243" s="11"/>
       <c r="G243" s="11"/>
       <c r="H243" s="11"/>
     </row>
-    <row r="244" spans="1:8" ht="32.1" customHeight="1">
+    <row r="244" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A244" s="8">
         <v>242</v>
       </c>
@@ -9215,119 +9607,135 @@
       <c r="G244" s="11"/>
       <c r="H244" s="11"/>
     </row>
-    <row r="245" spans="1:8" ht="32.1" customHeight="1">
+    <row r="245" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A245" s="8">
         <v>243</v>
       </c>
       <c r="B245" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="C245" s="12"/>
+      <c r="C245" s="19" t="s">
+        <v>517</v>
+      </c>
       <c r="D245" s="11"/>
       <c r="E245" s="11"/>
       <c r="F245" s="11"/>
       <c r="G245" s="11"/>
       <c r="H245" s="11"/>
     </row>
-    <row r="246" spans="1:8" ht="44.1" customHeight="1">
+    <row r="246" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A246" s="8">
         <v>244</v>
       </c>
       <c r="B246" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="C246" s="12"/>
+      <c r="C246" s="17" t="s">
+        <v>518</v>
+      </c>
       <c r="D246" s="11"/>
       <c r="E246" s="11"/>
       <c r="F246" s="11"/>
       <c r="G246" s="11"/>
       <c r="H246" s="11"/>
     </row>
-    <row r="247" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="247" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A247" s="8">
         <v>245</v>
       </c>
       <c r="B247" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="C247" s="12"/>
+      <c r="C247" s="17" t="s">
+        <v>519</v>
+      </c>
       <c r="D247" s="11"/>
       <c r="E247" s="11"/>
       <c r="F247" s="11"/>
       <c r="G247" s="11"/>
       <c r="H247" s="11"/>
     </row>
-    <row r="248" spans="1:8" ht="44.1" customHeight="1">
+    <row r="248" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A248" s="8">
         <v>246</v>
       </c>
       <c r="B248" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="C248" s="12"/>
+      <c r="C248" s="17" t="s">
+        <v>520</v>
+      </c>
       <c r="D248" s="11"/>
       <c r="E248" s="11"/>
       <c r="F248" s="11"/>
       <c r="G248" s="11"/>
       <c r="H248" s="11"/>
     </row>
-    <row r="249" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="249" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A249" s="8">
         <v>247</v>
       </c>
       <c r="B249" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="C249" s="12"/>
+      <c r="C249" s="17" t="s">
+        <v>521</v>
+      </c>
       <c r="D249" s="11"/>
       <c r="E249" s="11"/>
       <c r="F249" s="11"/>
       <c r="G249" s="11"/>
       <c r="H249" s="11"/>
     </row>
-    <row r="250" spans="1:8" ht="32.1" customHeight="1">
+    <row r="250" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A250" s="8">
         <v>248</v>
       </c>
       <c r="B250" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="C250" s="12"/>
+      <c r="C250" s="17" t="s">
+        <v>522</v>
+      </c>
       <c r="D250" s="11"/>
       <c r="E250" s="11"/>
       <c r="F250" s="11"/>
       <c r="G250" s="11"/>
       <c r="H250" s="11"/>
     </row>
-    <row r="251" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="251" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A251" s="8">
         <v>249</v>
       </c>
       <c r="B251" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C251" s="12"/>
+      <c r="C251" s="17" t="s">
+        <v>523</v>
+      </c>
       <c r="D251" s="11"/>
       <c r="E251" s="11"/>
       <c r="F251" s="11"/>
       <c r="G251" s="11"/>
       <c r="H251" s="11"/>
     </row>
-    <row r="252" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="252" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A252" s="8">
         <v>250</v>
       </c>
       <c r="B252" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="C252" s="12"/>
+      <c r="C252" s="17" t="s">
+        <v>524</v>
+      </c>
       <c r="D252" s="11"/>
       <c r="E252" s="11"/>
       <c r="F252" s="11"/>
       <c r="G252" s="11"/>
       <c r="H252" s="11"/>
     </row>
-    <row r="253" spans="1:8" ht="32.1" customHeight="1">
+    <row r="253" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A253" s="8">
         <v>251</v>
       </c>
@@ -9341,7 +9749,7 @@
       <c r="G253" s="11"/>
       <c r="H253" s="11"/>
     </row>
-    <row r="254" spans="1:8" ht="32.1" customHeight="1">
+    <row r="254" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A254" s="8">
         <v>252</v>
       </c>
@@ -9355,7 +9763,7 @@
       <c r="G254" s="11"/>
       <c r="H254" s="11"/>
     </row>
-    <row r="255" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="255" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A255" s="8">
         <v>253</v>
       </c>
@@ -9369,7 +9777,7 @@
       <c r="G255" s="11"/>
       <c r="H255" s="11"/>
     </row>
-    <row r="256" spans="1:8" ht="32.1" customHeight="1">
+    <row r="256" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A256" s="8">
         <v>254</v>
       </c>
@@ -9383,7 +9791,7 @@
       <c r="G256" s="11"/>
       <c r="H256" s="11"/>
     </row>
-    <row r="257" spans="1:8" ht="32.1" customHeight="1">
+    <row r="257" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A257" s="8">
         <v>255</v>
       </c>
@@ -9397,7 +9805,7 @@
       <c r="G257" s="11"/>
       <c r="H257" s="11"/>
     </row>
-    <row r="258" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="258" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A258" s="8">
         <v>256</v>
       </c>
@@ -9411,7 +9819,7 @@
       <c r="G258" s="11"/>
       <c r="H258" s="11"/>
     </row>
-    <row r="259" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="259" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A259" s="8">
         <v>257</v>
       </c>
@@ -9425,7 +9833,7 @@
       <c r="G259" s="11"/>
       <c r="H259" s="11"/>
     </row>
-    <row r="260" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="260" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A260" s="8">
         <v>258</v>
       </c>
@@ -9439,7 +9847,7 @@
       <c r="G260" s="11"/>
       <c r="H260" s="11"/>
     </row>
-    <row r="261" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="261" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A261" s="8">
         <v>259</v>
       </c>
@@ -9453,7 +9861,7 @@
       <c r="G261" s="11"/>
       <c r="H261" s="11"/>
     </row>
-    <row r="262" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="262" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A262" s="8">
         <v>260</v>
       </c>
@@ -9467,7 +9875,7 @@
       <c r="G262" s="11"/>
       <c r="H262" s="11"/>
     </row>
-    <row r="263" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="263" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A263" s="8">
         <v>261</v>
       </c>
@@ -9481,7 +9889,7 @@
       <c r="G263" s="11"/>
       <c r="H263" s="11"/>
     </row>
-    <row r="264" spans="1:8" ht="44.1" customHeight="1">
+    <row r="264" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A264" s="8">
         <v>262</v>
       </c>
@@ -9495,7 +9903,7 @@
       <c r="G264" s="11"/>
       <c r="H264" s="11"/>
     </row>
-    <row r="265" spans="1:8" ht="32.1" customHeight="1">
+    <row r="265" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A265" s="8">
         <v>263</v>
       </c>
@@ -9509,7 +9917,7 @@
       <c r="G265" s="11"/>
       <c r="H265" s="11"/>
     </row>
-    <row r="266" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="266" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A266" s="8">
         <v>264</v>
       </c>
@@ -9523,7 +9931,7 @@
       <c r="G266" s="11"/>
       <c r="H266" s="11"/>
     </row>
-    <row r="267" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="267" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A267" s="8">
         <v>265</v>
       </c>
@@ -9537,7 +9945,7 @@
       <c r="G267" s="11"/>
       <c r="H267" s="11"/>
     </row>
-    <row r="268" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="268" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A268" s="8">
         <v>266</v>
       </c>
@@ -9551,7 +9959,7 @@
       <c r="G268" s="11"/>
       <c r="H268" s="11"/>
     </row>
-    <row r="269" spans="1:8" ht="32.1" customHeight="1">
+    <row r="269" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A269" s="8">
         <v>267</v>
       </c>
@@ -9565,7 +9973,7 @@
       <c r="G269" s="11"/>
       <c r="H269" s="11"/>
     </row>
-    <row r="270" spans="1:8" ht="44.1" customHeight="1">
+    <row r="270" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A270" s="8">
         <v>268</v>
       </c>
@@ -9579,7 +9987,7 @@
       <c r="G270" s="11"/>
       <c r="H270" s="11"/>
     </row>
-    <row r="271" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="271" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A271" s="8">
         <v>269</v>
       </c>
@@ -9593,7 +10001,7 @@
       <c r="G271" s="11"/>
       <c r="H271" s="11"/>
     </row>
-    <row r="272" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="272" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A272" s="8">
         <v>270</v>
       </c>
@@ -9607,7 +10015,7 @@
       <c r="G272" s="11"/>
       <c r="H272" s="11"/>
     </row>
-    <row r="273" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="273" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A273" s="8">
         <v>271</v>
       </c>
@@ -9621,7 +10029,7 @@
       <c r="G273" s="11"/>
       <c r="H273" s="11"/>
     </row>
-    <row r="274" spans="1:8" ht="32.1" customHeight="1">
+    <row r="274" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A274" s="8">
         <v>272</v>
       </c>
@@ -9635,7 +10043,7 @@
       <c r="G274" s="11"/>
       <c r="H274" s="11"/>
     </row>
-    <row r="275" spans="1:8" ht="32.1" customHeight="1">
+    <row r="275" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A275" s="8">
         <v>273</v>
       </c>
@@ -9649,7 +10057,7 @@
       <c r="G275" s="11"/>
       <c r="H275" s="11"/>
     </row>
-    <row r="276" spans="1:8" ht="32.1" customHeight="1">
+    <row r="276" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A276" s="8">
         <v>274</v>
       </c>
@@ -9663,7 +10071,7 @@
       <c r="G276" s="11"/>
       <c r="H276" s="11"/>
     </row>
-    <row r="277" spans="1:8" ht="32.1" customHeight="1">
+    <row r="277" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A277" s="8">
         <v>275</v>
       </c>
@@ -9677,7 +10085,7 @@
       <c r="G277" s="11"/>
       <c r="H277" s="11"/>
     </row>
-    <row r="278" spans="1:8" ht="44.1" customHeight="1">
+    <row r="278" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A278" s="8">
         <v>276</v>
       </c>
@@ -9691,7 +10099,7 @@
       <c r="G278" s="11"/>
       <c r="H278" s="11"/>
     </row>
-    <row r="279" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="279" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A279" s="8">
         <v>277</v>
       </c>
@@ -9705,7 +10113,7 @@
       <c r="G279" s="11"/>
       <c r="H279" s="11"/>
     </row>
-    <row r="280" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="280" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A280" s="8">
         <v>278</v>
       </c>
@@ -9719,7 +10127,7 @@
       <c r="G280" s="11"/>
       <c r="H280" s="11"/>
     </row>
-    <row r="281" spans="1:8" ht="32.1" customHeight="1">
+    <row r="281" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A281" s="8">
         <v>279</v>
       </c>
@@ -9733,7 +10141,7 @@
       <c r="G281" s="11"/>
       <c r="H281" s="11"/>
     </row>
-    <row r="282" spans="1:8" ht="32.1" customHeight="1">
+    <row r="282" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A282" s="8">
         <v>280</v>
       </c>
@@ -9747,7 +10155,7 @@
       <c r="G282" s="11"/>
       <c r="H282" s="11"/>
     </row>
-    <row r="283" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="283" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A283" s="8">
         <v>281</v>
       </c>
@@ -9761,7 +10169,7 @@
       <c r="G283" s="11"/>
       <c r="H283" s="11"/>
     </row>
-    <row r="284" spans="1:8" ht="32.1" customHeight="1">
+    <row r="284" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A284" s="8">
         <v>282</v>
       </c>
@@ -9775,7 +10183,7 @@
       <c r="G284" s="11"/>
       <c r="H284" s="11"/>
     </row>
-    <row r="285" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="285" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A285" s="8">
         <v>283</v>
       </c>
@@ -9789,7 +10197,7 @@
       <c r="G285" s="11"/>
       <c r="H285" s="11"/>
     </row>
-    <row r="286" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="286" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A286" s="8">
         <v>284</v>
       </c>
@@ -9803,7 +10211,7 @@
       <c r="G286" s="11"/>
       <c r="H286" s="11"/>
     </row>
-    <row r="287" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="287" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A287" s="8">
         <v>285</v>
       </c>
@@ -9817,7 +10225,7 @@
       <c r="G287" s="11"/>
       <c r="H287" s="11"/>
     </row>
-    <row r="288" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="288" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A288" s="8">
         <v>286</v>
       </c>
@@ -9831,7 +10239,7 @@
       <c r="G288" s="11"/>
       <c r="H288" s="11"/>
     </row>
-    <row r="289" spans="1:8" ht="32.1" customHeight="1">
+    <row r="289" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A289" s="8">
         <v>287</v>
       </c>
@@ -9845,7 +10253,7 @@
       <c r="G289" s="11"/>
       <c r="H289" s="11"/>
     </row>
-    <row r="290" spans="1:8" ht="32.1" customHeight="1">
+    <row r="290" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A290" s="8">
         <v>288</v>
       </c>
@@ -9859,7 +10267,7 @@
       <c r="G290" s="11"/>
       <c r="H290" s="11"/>
     </row>
-    <row r="291" spans="1:8" ht="44.1" customHeight="1">
+    <row r="291" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A291" s="8">
         <v>289</v>
       </c>
@@ -9873,7 +10281,7 @@
       <c r="G291" s="11"/>
       <c r="H291" s="11"/>
     </row>
-    <row r="292" spans="1:8" ht="32.1" customHeight="1">
+    <row r="292" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A292" s="8">
         <v>290</v>
       </c>
@@ -9887,7 +10295,7 @@
       <c r="G292" s="11"/>
       <c r="H292" s="11"/>
     </row>
-    <row r="293" spans="1:8" ht="32.1" customHeight="1">
+    <row r="293" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A293" s="8">
         <v>291</v>
       </c>
@@ -9901,7 +10309,7 @@
       <c r="G293" s="11"/>
       <c r="H293" s="11"/>
     </row>
-    <row r="294" spans="1:8" ht="32.1" customHeight="1">
+    <row r="294" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A294" s="8">
         <v>292</v>
       </c>
@@ -9915,7 +10323,7 @@
       <c r="G294" s="11"/>
       <c r="H294" s="11"/>
     </row>
-    <row r="295" spans="1:8" ht="32.1" customHeight="1">
+    <row r="295" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A295" s="8">
         <v>293</v>
       </c>
@@ -9929,7 +10337,7 @@
       <c r="G295" s="11"/>
       <c r="H295" s="11"/>
     </row>
-    <row r="296" spans="1:8" ht="44.1" customHeight="1">
+    <row r="296" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A296" s="8">
         <v>294</v>
       </c>
@@ -9943,7 +10351,7 @@
       <c r="G296" s="11"/>
       <c r="H296" s="11"/>
     </row>
-    <row r="297" spans="1:8" ht="32.1" customHeight="1">
+    <row r="297" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A297" s="8">
         <v>295</v>
       </c>
@@ -9957,7 +10365,7 @@
       <c r="G297" s="11"/>
       <c r="H297" s="11"/>
     </row>
-    <row r="298" spans="1:8" ht="44.1" customHeight="1">
+    <row r="298" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A298" s="8">
         <v>296</v>
       </c>
@@ -9971,7 +10379,7 @@
       <c r="G298" s="11"/>
       <c r="H298" s="11"/>
     </row>
-    <row r="299" spans="1:8" ht="32.1" customHeight="1">
+    <row r="299" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A299" s="8">
         <v>297</v>
       </c>
@@ -9985,7 +10393,7 @@
       <c r="G299" s="11"/>
       <c r="H299" s="11"/>
     </row>
-    <row r="300" spans="1:8" ht="32.1" customHeight="1">
+    <row r="300" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A300" s="8">
         <v>298</v>
       </c>
@@ -9999,7 +10407,7 @@
       <c r="G300" s="11"/>
       <c r="H300" s="11"/>
     </row>
-    <row r="301" spans="1:8" ht="32.1" customHeight="1">
+    <row r="301" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A301" s="8">
         <v>299</v>
       </c>
@@ -10013,7 +10421,7 @@
       <c r="G301" s="11"/>
       <c r="H301" s="11"/>
     </row>
-    <row r="302" spans="1:8" ht="44.1" customHeight="1">
+    <row r="302" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A302" s="8">
         <v>300</v>
       </c>
@@ -10027,7 +10435,7 @@
       <c r="G302" s="11"/>
       <c r="H302" s="11"/>
     </row>
-    <row r="303" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="303" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A303" s="8">
         <v>301</v>
       </c>
@@ -10041,7 +10449,7 @@
       <c r="G303" s="11"/>
       <c r="H303" s="11"/>
     </row>
-    <row r="304" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="304" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A304" s="8">
         <v>302</v>
       </c>
@@ -10055,7 +10463,7 @@
       <c r="G304" s="11"/>
       <c r="H304" s="11"/>
     </row>
-    <row r="305" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="305" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A305" s="8">
         <v>303</v>
       </c>
@@ -10069,7 +10477,7 @@
       <c r="G305" s="11"/>
       <c r="H305" s="11"/>
     </row>
-    <row r="306" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="306" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A306" s="8">
         <v>304</v>
       </c>
@@ -10083,7 +10491,7 @@
       <c r="G306" s="11"/>
       <c r="H306" s="11"/>
     </row>
-    <row r="307" spans="1:8" ht="32.1" customHeight="1">
+    <row r="307" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A307" s="8">
         <v>305</v>
       </c>
@@ -10097,7 +10505,7 @@
       <c r="G307" s="11"/>
       <c r="H307" s="11"/>
     </row>
-    <row r="308" spans="1:8" ht="32.1" customHeight="1">
+    <row r="308" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A308" s="8">
         <v>306</v>
       </c>
@@ -10111,7 +10519,7 @@
       <c r="G308" s="11"/>
       <c r="H308" s="11"/>
     </row>
-    <row r="309" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="309" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A309" s="8">
         <v>307</v>
       </c>
@@ -10125,7 +10533,7 @@
       <c r="G309" s="11"/>
       <c r="H309" s="11"/>
     </row>
-    <row r="310" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="310" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A310" s="8">
         <v>308</v>
       </c>
@@ -10139,7 +10547,7 @@
       <c r="G310" s="11"/>
       <c r="H310" s="11"/>
     </row>
-    <row r="311" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="311" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A311" s="8">
         <v>309</v>
       </c>
@@ -10153,7 +10561,7 @@
       <c r="G311" s="11"/>
       <c r="H311" s="11"/>
     </row>
-    <row r="312" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="312" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A312" s="8">
         <v>310</v>
       </c>
@@ -10167,7 +10575,7 @@
       <c r="G312" s="11"/>
       <c r="H312" s="11"/>
     </row>
-    <row r="313" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="313" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A313" s="8">
         <v>311</v>
       </c>
@@ -10181,7 +10589,7 @@
       <c r="G313" s="11"/>
       <c r="H313" s="11"/>
     </row>
-    <row r="314" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="314" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A314" s="8">
         <v>312</v>
       </c>
@@ -10195,7 +10603,7 @@
       <c r="G314" s="11"/>
       <c r="H314" s="11"/>
     </row>
-    <row r="315" spans="1:8" ht="32.1" customHeight="1">
+    <row r="315" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A315" s="8">
         <v>313</v>
       </c>
@@ -10209,7 +10617,7 @@
       <c r="G315" s="11"/>
       <c r="H315" s="11"/>
     </row>
-    <row r="316" spans="1:8" ht="32.1" customHeight="1">
+    <row r="316" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A316" s="8">
         <v>314</v>
       </c>
@@ -10223,7 +10631,7 @@
       <c r="G316" s="11"/>
       <c r="H316" s="11"/>
     </row>
-    <row r="317" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="317" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A317" s="8">
         <v>315</v>
       </c>
@@ -10237,7 +10645,7 @@
       <c r="G317" s="11"/>
       <c r="H317" s="11"/>
     </row>
-    <row r="318" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="318" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A318" s="8">
         <v>316</v>
       </c>
@@ -10251,7 +10659,7 @@
       <c r="G318" s="11"/>
       <c r="H318" s="11"/>
     </row>
-    <row r="319" spans="1:8" ht="32.1" customHeight="1">
+    <row r="319" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A319" s="8">
         <v>317</v>
       </c>
@@ -10265,7 +10673,7 @@
       <c r="G319" s="11"/>
       <c r="H319" s="11"/>
     </row>
-    <row r="320" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="320" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A320" s="8">
         <v>318</v>
       </c>
@@ -10279,7 +10687,7 @@
       <c r="G320" s="11"/>
       <c r="H320" s="11"/>
     </row>
-    <row r="321" spans="1:8" ht="32.1" customHeight="1">
+    <row r="321" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A321" s="8">
         <v>319</v>
       </c>
@@ -10293,7 +10701,7 @@
       <c r="G321" s="11"/>
       <c r="H321" s="11"/>
     </row>
-    <row r="322" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="322" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A322" s="8">
         <v>320</v>
       </c>
@@ -10307,7 +10715,7 @@
       <c r="G322" s="11"/>
       <c r="H322" s="11"/>
     </row>
-    <row r="323" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="323" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A323" s="8">
         <v>321</v>
       </c>
@@ -10321,7 +10729,7 @@
       <c r="G323" s="11"/>
       <c r="H323" s="11"/>
     </row>
-    <row r="324" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="324" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A324" s="8">
         <v>322</v>
       </c>
@@ -10335,7 +10743,7 @@
       <c r="G324" s="11"/>
       <c r="H324" s="11"/>
     </row>
-    <row r="325" spans="1:8" ht="32.1" customHeight="1">
+    <row r="325" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A325" s="8">
         <v>323</v>
       </c>
@@ -10349,7 +10757,7 @@
       <c r="G325" s="11"/>
       <c r="H325" s="11"/>
     </row>
-    <row r="326" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="326" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A326" s="8">
         <v>324</v>
       </c>
@@ -10363,7 +10771,7 @@
       <c r="G326" s="11"/>
       <c r="H326" s="11"/>
     </row>
-    <row r="327" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="327" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A327" s="8">
         <v>325</v>
       </c>
@@ -10377,7 +10785,7 @@
       <c r="G327" s="11"/>
       <c r="H327" s="11"/>
     </row>
-    <row r="328" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="328" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A328" s="8">
         <v>326</v>
       </c>
@@ -10391,7 +10799,7 @@
       <c r="G328" s="11"/>
       <c r="H328" s="11"/>
     </row>
-    <row r="329" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="329" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A329" s="8">
         <v>327</v>
       </c>
@@ -10405,7 +10813,7 @@
       <c r="G329" s="11"/>
       <c r="H329" s="11"/>
     </row>
-    <row r="330" spans="1:8" ht="32.1" customHeight="1">
+    <row r="330" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A330" s="8">
         <v>328</v>
       </c>
@@ -10419,7 +10827,7 @@
       <c r="G330" s="11"/>
       <c r="H330" s="11"/>
     </row>
-    <row r="331" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="331" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A331" s="8">
         <v>329</v>
       </c>
@@ -10433,7 +10841,7 @@
       <c r="G331" s="11"/>
       <c r="H331" s="11"/>
     </row>
-    <row r="332" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="332" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A332" s="8">
         <v>330</v>
       </c>
@@ -10447,7 +10855,7 @@
       <c r="G332" s="11"/>
       <c r="H332" s="11"/>
     </row>
-    <row r="333" spans="1:8" ht="32.1" customHeight="1">
+    <row r="333" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A333" s="8">
         <v>331</v>
       </c>
@@ -10461,7 +10869,7 @@
       <c r="G333" s="11"/>
       <c r="H333" s="11"/>
     </row>
-    <row r="334" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="334" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A334" s="8">
         <v>332</v>
       </c>
@@ -10475,7 +10883,7 @@
       <c r="G334" s="11"/>
       <c r="H334" s="11"/>
     </row>
-    <row r="335" spans="1:8" ht="32.1" customHeight="1">
+    <row r="335" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A335" s="8">
         <v>333</v>
       </c>

</xml_diff>